<commit_message>
reporte 13/04 - 19/04
</commit_message>
<xml_diff>
--- a/public/reports/Reporte_Avenue_Napoles.xlsx
+++ b/public/reports/Reporte_Avenue_Napoles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergirams/Development/Kiper/backend/apikiper/public/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0ACDF93E-26F0-3B41-B6F5-84390725D3A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF26C910-87D1-104D-9351-4A9276728217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="13940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27480" yWindow="460" windowWidth="34720" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="192">
   <si>
     <t>A</t>
   </si>
@@ -137,588 +137,484 @@
     <t>Alejandra Campos García</t>
   </si>
   <si>
-    <t>2020-04-12 14:55:52</t>
-  </si>
-  <si>
-    <t>2020-04-12 14:31:36</t>
-  </si>
-  <si>
-    <t>2020-04-12 13:15:30</t>
-  </si>
-  <si>
-    <t>2020-04-12 02:50:53</t>
-  </si>
-  <si>
-    <t>2020-04-11 23:29:04</t>
-  </si>
-  <si>
-    <t>2020-04-11 22:14:41</t>
-  </si>
-  <si>
-    <t>2020-04-11 21:38:57</t>
-  </si>
-  <si>
-    <t>2020-04-11 19:43:22</t>
-  </si>
-  <si>
-    <t>2020-04-11 17:30:37</t>
-  </si>
-  <si>
-    <t>2020-04-11 16:17:07</t>
-  </si>
-  <si>
-    <t>2020-04-11 11:54:37</t>
-  </si>
-  <si>
-    <t>2020-04-11 09:43:49</t>
-  </si>
-  <si>
-    <t>2020-04-11 01:23:05</t>
-  </si>
-  <si>
-    <t>2020-04-11 00:08:14</t>
-  </si>
-  <si>
-    <t>2020-04-10 20:26:28</t>
-  </si>
-  <si>
-    <t>2020-04-10 17:27:36</t>
-  </si>
-  <si>
-    <t>2020-04-10 15:57:17</t>
-  </si>
-  <si>
-    <t>2020-04-10 10:05:13</t>
-  </si>
-  <si>
-    <t>2020-04-10 10:02:24</t>
-  </si>
-  <si>
-    <t>2020-04-10 03:24:03</t>
-  </si>
-  <si>
-    <t>2020-04-10 01:57:52</t>
-  </si>
-  <si>
-    <t>2020-04-09 23:31:16</t>
-  </si>
-  <si>
-    <t>2020-04-09 15:21:43</t>
-  </si>
-  <si>
-    <t>2020-04-09 13:51:03</t>
-  </si>
-  <si>
-    <t>2020-04-09 13:41:45</t>
-  </si>
-  <si>
-    <t>2020-04-09 12:18:11</t>
-  </si>
-  <si>
-    <t>2020-04-09 11:02:51</t>
-  </si>
-  <si>
-    <t>2020-04-09 10:56:53</t>
-  </si>
-  <si>
-    <t>2020-04-09 10:33:30</t>
-  </si>
-  <si>
-    <t>2020-04-09 10:06:54</t>
-  </si>
-  <si>
-    <t>2020-04-08 23:29:38</t>
-  </si>
-  <si>
-    <t>2020-04-08 17:05:44</t>
-  </si>
-  <si>
-    <t>2020-04-08 13:19:58</t>
-  </si>
-  <si>
-    <t>2020-04-08 13:00:53</t>
-  </si>
-  <si>
-    <t>2020-04-08 08:50:56</t>
-  </si>
-  <si>
-    <t>2020-04-08 02:09:21</t>
-  </si>
-  <si>
-    <t>2020-04-07 20:10:13</t>
-  </si>
-  <si>
-    <t>2020-04-07 16:03:01</t>
-  </si>
-  <si>
-    <t>2020-04-07 12:30:01</t>
-  </si>
-  <si>
-    <t>2020-04-07 09:24:24</t>
-  </si>
-  <si>
-    <t>2020-04-07 02:40:25</t>
-  </si>
-  <si>
-    <t>2020-04-06 23:27:38</t>
-  </si>
-  <si>
-    <t>2020-04-06 20:12:25</t>
-  </si>
-  <si>
-    <t>2020-04-06 16:01:42</t>
-  </si>
-  <si>
-    <t>2020-04-06 13:44:26</t>
-  </si>
-  <si>
-    <t>2020-04-06 11:20:14</t>
-  </si>
-  <si>
-    <t>2020-04-06 02:25:37</t>
-  </si>
-  <si>
-    <t>2020-04-06 02:03:13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zayani Pantoja Alcantar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sandra Hernandez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Andrea </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Francisco </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gilberto Salas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juan Carlos Tirado </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heriberto Flores Vazquez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaryCar Becrril </t>
-  </si>
-  <si>
-    <t xml:space="preserve">China SG </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carlos tomás </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carlos Cesar Tepale </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enrique López </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emmanuel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ricardo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arnulfo Perez Uzeta </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fernando González </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alex Guti Locken </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patricia Martínez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omar Ortiz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laura iran </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alejandro Jonathan Martínez Martínez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natalia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sinaí Mota </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARIA EUGENIA GUILLEN </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eva Lopez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jorge Martínez Hernández </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isabel bolivar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jose Luis Oliveros Garcia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miriam Rg </t>
-  </si>
-  <si>
-    <t>Valeria Torres Ramirez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erika Hernandez Jimenez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alexander </t>
-  </si>
-  <si>
-    <t>Ricardo Rivera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeanette tapia flores </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geraldin Mendoza </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noemi Gomez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javier Marin Zurita </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haméd Sahíd </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beatriz Guerrero </t>
-  </si>
-  <si>
-    <t xml:space="preserve">alejandro mendoza </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valeria Núñez Peralta </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erika </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guillermo Sanchez Mendez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antonio Carrillo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virginia Bernardini </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jeshua Rosiles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Itzia Torres Alarcón </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mónica Romero </t>
-  </si>
-  <si>
-    <t>zayapantoja@hotmail.com</t>
-  </si>
-  <si>
-    <t>Sandycasal@yahoo.com.mx</t>
-  </si>
-  <si>
-    <t>andrea.glz95@hotmail.com</t>
-  </si>
-  <si>
-    <t>pacon9201@gmail.com</t>
-  </si>
-  <si>
-    <t>gsalas@nev.mx</t>
-  </si>
-  <si>
-    <t>juanc.tiradoc@gmail.com</t>
-  </si>
-  <si>
-    <t>heribertoflores1@yahoo.com.mx</t>
-  </si>
-  <si>
-    <t>mary.blen@hotmail.com</t>
-  </si>
-  <si>
-    <t>anaid.gilda@gmail.com</t>
-  </si>
-  <si>
-    <t>carlostomasramos@icloud.com</t>
-  </si>
-  <si>
-    <t>cctepale@yahoo.com.mx</t>
-  </si>
-  <si>
-    <t>enrilole@gmail.com</t>
-  </si>
-  <si>
-    <t>em_gar_her@live.com.mx</t>
-  </si>
-  <si>
-    <t>adrianmendezsoto@hotmail.com</t>
-  </si>
-  <si>
-    <t>arpeuz@yahoo.com</t>
-  </si>
-  <si>
-    <t>fernandogs63@gmail.com</t>
-  </si>
-  <si>
-    <t>aguriwrrws@zegna.com</t>
-  </si>
-  <si>
-    <t>p.martinezdavila02@gmail.com</t>
-  </si>
-  <si>
-    <t>Chinoac21@gmail.com</t>
-  </si>
-  <si>
-    <t>wiwi.esp.ls@gmail.com</t>
-  </si>
-  <si>
-    <t>jounasmtz@gmail.com</t>
-  </si>
-  <si>
-    <t>natytellez-1994@hotmail.com</t>
-  </si>
-  <si>
-    <t>sinaimotacatayjuan@gmail.com</t>
-  </si>
-  <si>
-    <t>PAMINORIEGA@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>eva.enturia@yahoo.com.mx</t>
-  </si>
-  <si>
-    <t>mhzjorge@gmail.com</t>
-  </si>
-  <si>
-    <t>mibolivarc@gmail.com</t>
-  </si>
-  <si>
-    <t>joseoliveros@uriel.edu.mx</t>
-  </si>
-  <si>
-    <t>lic.miriamrosado@gmail.com</t>
-  </si>
-  <si>
-    <t>valeria.torres.rmz@outlook.com</t>
-  </si>
-  <si>
-    <t>ehernandezj@invex.com</t>
-  </si>
-  <si>
-    <t>alexandernavarroperez@gmail.com</t>
-  </si>
-  <si>
-    <t>ricardo.rivera@begrand.mx</t>
-  </si>
-  <si>
-    <t>jeantf03@gmail.com</t>
-  </si>
-  <si>
-    <t>Gerii2309@hotmail.com</t>
-  </si>
-  <si>
-    <t>yth@gmail.com</t>
-  </si>
-  <si>
-    <t>Marinjavier@yahoo.com</t>
-  </si>
-  <si>
-    <t>sahid_m@hotmail.com</t>
-  </si>
-  <si>
-    <t>gvbeatriz59@gmail.com</t>
-  </si>
-  <si>
-    <t>planeacion15@gmail.com</t>
-  </si>
-  <si>
-    <t>valerianpkarate@gmail.com</t>
-  </si>
-  <si>
-    <t>erikterve@icloud.com</t>
-  </si>
-  <si>
-    <t>gsanmen13@gmail.com</t>
-  </si>
-  <si>
-    <t>draxon17@gmail.com</t>
-  </si>
-  <si>
-    <t>virber@hotmail.com</t>
-  </si>
-  <si>
-    <t>jmr.designer@hotmail.com</t>
-  </si>
-  <si>
-    <t>itziammaria@gmail.com</t>
-  </si>
-  <si>
-    <t>monromero20@gmail.com</t>
-  </si>
-  <si>
-    <t>Se equivocó creia que el proyecto estaba en Guadalajara</t>
-  </si>
-  <si>
-    <t>Trae presupuesto de $3,000,000 de pesos</t>
-  </si>
-  <si>
-    <t>Teléfono y e-mail equivocado. Me contestó y me dice que tomaron sus datos sin su permiso.</t>
-  </si>
-  <si>
-    <t>No contesta se le envía información general por whats y por mail.</t>
-  </si>
-  <si>
-    <t>No contesta entra buzón, se le envió mail de presentación y cotización de departamentos de 2 y 3 recamaras</t>
-  </si>
-  <si>
-    <t>Fuera de presupuesto trae $3,500.000 de pesos</t>
-  </si>
-  <si>
-    <t>No contesta entra buzón. Se le envió mail de presentación y cotización de departamentos de 2 y 3 recamaras</t>
-  </si>
-  <si>
-    <t>No contesta, se le envió mail de presentación y cotización de departamentos de 2 y 3 recamaras</t>
-  </si>
-  <si>
-    <t>El teléfono que dejó solo cuenta con servicio para navegar en internet, se le envía información general por mail</t>
-  </si>
-  <si>
-    <t>No toma llamadas, le envie whats y mail con información general del proyecto.</t>
-  </si>
-  <si>
-    <t>Tiene presupuesto bajo $4M pero solicito información general y cotización del 205B</t>
-  </si>
-  <si>
-    <t>Teléfono equivocado. Se le envió mail de presentación y cotización de departamentos de 2 y 3 recamaras.</t>
-  </si>
-  <si>
-    <t>Numero no disponible, se envía información general por mail</t>
-  </si>
-  <si>
-    <t>El telefono no existe se le envía información general  por mail</t>
-  </si>
-  <si>
-    <t>Busca 3 recamaras, no quiso dar presupuesto, se le envía 403C.
+    <t>2020-04-19 17:33:40</t>
+  </si>
+  <si>
+    <t>2020-04-19 17:09:05</t>
+  </si>
+  <si>
+    <t>2020-04-19 13:20:42</t>
+  </si>
+  <si>
+    <t>2020-04-19 11:43:05</t>
+  </si>
+  <si>
+    <t>2020-04-19 01:21:04</t>
+  </si>
+  <si>
+    <t>2020-04-18 18:56:18</t>
+  </si>
+  <si>
+    <t>2020-04-18 11:54:19</t>
+  </si>
+  <si>
+    <t>2020-04-18 11:22:06</t>
+  </si>
+  <si>
+    <t>2020-04-18 00:37:06</t>
+  </si>
+  <si>
+    <t>2020-04-17 22:11:30</t>
+  </si>
+  <si>
+    <t>2020-04-17 20:28:21</t>
+  </si>
+  <si>
+    <t>2020-04-17 15:08:09</t>
+  </si>
+  <si>
+    <t>2020-04-17 10:11:25</t>
+  </si>
+  <si>
+    <t>2020-04-16 23:47:54</t>
+  </si>
+  <si>
+    <t>2020-04-16 21:59:41</t>
+  </si>
+  <si>
+    <t>2020-04-16 19:20:49</t>
+  </si>
+  <si>
+    <t>2020-04-16 13:41:50</t>
+  </si>
+  <si>
+    <t>2020-04-15 22:34:38</t>
+  </si>
+  <si>
+    <t>2020-04-15 21:54:44</t>
+  </si>
+  <si>
+    <t>2020-04-15 17:48:40</t>
+  </si>
+  <si>
+    <t>2020-04-15 14:29:39</t>
+  </si>
+  <si>
+    <t>2020-04-15 07:40:48</t>
+  </si>
+  <si>
+    <t>2020-04-15 00:21:10</t>
+  </si>
+  <si>
+    <t>2020-04-14 22:47:19</t>
+  </si>
+  <si>
+    <t>2020-04-14 22:32:59</t>
+  </si>
+  <si>
+    <t>2020-04-14 17:18:17</t>
+  </si>
+  <si>
+    <t>2020-04-14 12:53:15</t>
+  </si>
+  <si>
+    <t>2020-04-14 12:38:17</t>
+  </si>
+  <si>
+    <t>2020-04-14 08:02:26</t>
+  </si>
+  <si>
+    <t>2020-04-14 07:12:10</t>
+  </si>
+  <si>
+    <t>2020-04-14 01:39:59</t>
+  </si>
+  <si>
+    <t>2020-04-13 23:58:11</t>
+  </si>
+  <si>
+    <t>2020-04-13 22:41:25</t>
+  </si>
+  <si>
+    <t>2020-04-13 19:38:20</t>
+  </si>
+  <si>
+    <t>2020-04-13 16:00:41</t>
+  </si>
+  <si>
+    <t>2020-04-13 15:34:29</t>
+  </si>
+  <si>
+    <t>2020-04-13 14:45:34</t>
+  </si>
+  <si>
+    <t>2020-04-13 13:00:02</t>
+  </si>
+  <si>
+    <t>2020-04-13 12:55:29</t>
+  </si>
+  <si>
+    <t>2020-04-13 11:35:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lizbeth Becerril Contreras </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alicia Gtz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerardo Marin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melissa Alvarez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuria Yunuen </t>
+  </si>
+  <si>
+    <t>Edgar Salas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carmina Rodriguez Zaldivar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ilse Nayeli </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midori abigail silva Reyes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tania Annirack Flores García </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mafalda Comales </t>
+  </si>
+  <si>
+    <t>Elizabeth Gonzalez</t>
+  </si>
+  <si>
+    <t>Diana Aline Garcia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuri Sevilla </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samantha Shs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jose Fragoso </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brayan Valdes Vazquez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diego Trujillo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alejandro Rivera centeno </t>
+  </si>
+  <si>
+    <t>Jesus Andres Garcia Medina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roberto Gonzalez Labastida </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marco </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adriana Islas Romero </t>
+  </si>
+  <si>
+    <t xml:space="preserve">María Esmeralda Lopez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana Aguirre </t>
+  </si>
+  <si>
+    <t>Luis Gonzalez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garbu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alan Amador Perez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guadalupe Cárdenas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">marco antonio Ramírez Ortiz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elizabeth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atlantida Resendiz Cruz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grace Izquierdo Molleda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noel Acosta </t>
+  </si>
+  <si>
+    <t>Mariana Ituarte</t>
+  </si>
+  <si>
+    <t>Manuel Dovali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jennifer </t>
+  </si>
+  <si>
+    <t>lbecerril018@gmail.com</t>
+  </si>
+  <si>
+    <t>alizzgo_78@hotmail.com</t>
+  </si>
+  <si>
+    <t>gmarin2000@hotmail.com</t>
+  </si>
+  <si>
+    <t>Mel-alvarez@hotmail.com</t>
+  </si>
+  <si>
+    <t>nuria_y_om@icloud.com</t>
+  </si>
+  <si>
+    <t>edgar_salas@hotmail.com</t>
+  </si>
+  <si>
+    <t>crodriguezzsldivar@gmail.com</t>
+  </si>
+  <si>
+    <t>ilse3571@hotmail.com</t>
+  </si>
+  <si>
+    <t>silvamidori986@gmail.com</t>
+  </si>
+  <si>
+    <t>maradan.tr@gmail.com</t>
+  </si>
+  <si>
+    <t>Pilrcr@hotmail.com</t>
+  </si>
+  <si>
+    <t>elypope200879@gmail.com</t>
+  </si>
+  <si>
+    <t>alinearteaga@me.com</t>
+  </si>
+  <si>
+    <t>yurisevilla@hotmail.com</t>
+  </si>
+  <si>
+    <t>shsondersam90@hotmail.com</t>
+  </si>
+  <si>
+    <t>Jofrago1302@gmail.com</t>
+  </si>
+  <si>
+    <t>valdesvzquezbrayan@gmail.com</t>
+  </si>
+  <si>
+    <t>dtrujillovaz@gmail.com</t>
+  </si>
+  <si>
+    <t>alejandro_1508@outlook.com</t>
+  </si>
+  <si>
+    <t>acmituarte@yahoo.com.mx</t>
+  </si>
+  <si>
+    <t>jesus_andres_14@hotmail.com</t>
+  </si>
+  <si>
+    <t>rogola66@live.com.mx</t>
+  </si>
+  <si>
+    <t>marcoar.galan@gmail.com</t>
+  </si>
+  <si>
+    <t>adry.islas@hotmail.com</t>
+  </si>
+  <si>
+    <t>mariaesmerald@yahoo.com</t>
+  </si>
+  <si>
+    <t>ann1323.aa@gmail.com</t>
+  </si>
+  <si>
+    <t>5539334916@phonecall.com</t>
+  </si>
+  <si>
+    <t>garbiecheverria4@gmail.com</t>
+  </si>
+  <si>
+    <t>andres.michelr@gmail.com</t>
+  </si>
+  <si>
+    <t>alanamador7@gmail.com</t>
+  </si>
+  <si>
+    <t>lucardenasgtz@gmail.com</t>
+  </si>
+  <si>
+    <t>marckram9@gmail.com</t>
+  </si>
+  <si>
+    <t>Wvc8s7SPa@outlook.com</t>
+  </si>
+  <si>
+    <t>martinidasa@yahoo.com</t>
+  </si>
+  <si>
+    <t>atlantida.resendiz@gmail.com</t>
+  </si>
+  <si>
+    <t>molledag@hotmail.com</t>
+  </si>
+  <si>
+    <t>noel.acosta17@gmail.com</t>
+  </si>
+  <si>
+    <t>ituartemariana@gmail.com</t>
+  </si>
+  <si>
+    <t>manuel.dovali@gmail.com</t>
+  </si>
+  <si>
+    <t>Jennygaray14102000@gmail.com</t>
+  </si>
+  <si>
+    <t>No contesta, se le envió mail de presentación y cotizaciones de departamentos de 2 y 3 recamaras.
+SEguimiento</t>
+  </si>
+  <si>
+    <t>No contesta telefono se le envía información general por mail</t>
+  </si>
+  <si>
+    <t>Le llamé y me dice que primero le envíe la información del proyecto y cotización de 2 y 3 recamara para que los revise.
 Seguimiento</t>
   </si>
   <si>
-    <t>Entra buzón se le envia mensaje por whats e información general por mail.</t>
-  </si>
-  <si>
-    <t>No contesta, entra buzón a la primera,se le envía mail de presentación.
+    <t>Visita al Showroom el sábado de 18 de Abril, se llevo información del 307A Llamarle el lunes 20</t>
+  </si>
+  <si>
+    <t>No contesta, entra buzón. se le envió mail de presentación y cotizaciones de departamentos de 2 y 3 recamaras.
 Seguimiento</t>
   </si>
   <si>
-    <t>Busca en renta, pero solicito cotización del 205B</t>
-  </si>
-  <si>
-    <t>Esta buscando en renta</t>
-  </si>
-  <si>
-    <t>Es corredora y esta buscando para su hijo Rodrigo Velázquez Guillen y le interesa el PH03C. Se le envía cotización.
+    <t>Entra buzón se le envía información general por mail.</t>
+  </si>
+  <si>
+    <t>Busca 2 recamaras y tiene hasta $7 millones. Se le envió cotización del 205B
 Seguimiento</t>
   </si>
   <si>
-    <t>Entra siempre buzon se le envía información general por mail</t>
-  </si>
-  <si>
-    <t>Busca de 2 y 3 recamaras. no me dijo presupuesto. Se le envió cotización del 205B y 403C</t>
-  </si>
-  <si>
-    <t>No contesta se le envía información general por mail</t>
-  </si>
-  <si>
-    <t>Me contesta y cuelga. no logro comunicarme con el cliente.
-Se le envía mail de presentación.
+    <t>Se le envía información de 3 recamaras por whats y Tiene cita programada para el Jueves 23 de Abril</t>
+  </si>
+  <si>
+    <t>Solicitó informes del proyecto y cotización de departamentos de 2 recamaras. Se le envió cotización del 205B. Seguimiento</t>
+  </si>
+  <si>
+    <t>Solicito información general por whats.</t>
+  </si>
+  <si>
+    <t>Fuera de presupuesto trae $4,500,000</t>
+  </si>
+  <si>
+    <t>No contesta, entra buzón. Se le envió mail de presentación y cotizaciones de 2 y 3 recamaras.
 Seguimiento</t>
   </si>
   <si>
-    <t>Solicita información de 3 recamaras, esta empezando a ver</t>
-  </si>
-  <si>
-    <t>Envié cotización de PH3A y PH1C y rango de precios de deptos</t>
-  </si>
-  <si>
-    <t>Trae presupuesto hasta $5,000,000 peso que le mande información</t>
-  </si>
-  <si>
-    <t>Presupuesto bajo $3.4M</t>
-  </si>
-  <si>
-    <t>Es corredor, traerá clientes.</t>
-  </si>
-  <si>
-    <t>No contesta, entra buzón se le envía mail de presentación.
+    <t>Me solicitó informes de PH's: PH02A, PU06A, PH09A y PH10A</t>
+  </si>
+  <si>
+    <t>Entra buzón a la primera. Se le envió mail de presentación y cotizaciones de 2 y 3 recamaras.
 Seguimiento</t>
   </si>
   <si>
-    <t>Trae presupuesto de $4,000,000 sin embardo quiere que le mande información de 2 recamaras para verlo</t>
-  </si>
-  <si>
-    <t>Dejó teléfono equivocado, se le envió mail de presentación. 
-Seguimiento por mail.</t>
-  </si>
-  <si>
-    <t>Busca de 2 y 3 recamaras para inversión.
+    <t>Busca en Renta</t>
+  </si>
+  <si>
+    <t>Buzón de voz, se le envía información general por mail.</t>
+  </si>
+  <si>
+    <t>No dejo No. telefónico. Se le envía mail de presentación y cotización de 2 y 3 recamaras.
+Seguimiento por mail</t>
+  </si>
+  <si>
+    <t>El teléfono no sta disponible, se envía información general por mail.</t>
+  </si>
+  <si>
+    <t>No contesta, entra buzón. Se le envió mail de presentación y cotización de 2 y 3 recamaras. Seguimiento</t>
+  </si>
+  <si>
+    <t>Se les envía información de 2 y 3 recamaras a ella y a su esposo Diego Castillo</t>
+  </si>
+  <si>
+    <t>Me contacta para pedir mi iopinión sobre otros desarrollos que ha visto en Condesa y Roma, le ofrezco también Av Napoles</t>
+  </si>
+  <si>
+    <t>Cuelga el teléfono, se le envía información general por whats y por mail</t>
+  </si>
+  <si>
+    <t>Busca departamento exterior de 2 recamaras se le enviaron los modelos 8C y 8A.
 Seguimiento</t>
   </si>
   <si>
-    <t>Entra buzón se le envía información por mail</t>
-  </si>
-  <si>
-    <t>Entra buzón. Se le envía mail de presentación.
-SEguimiento</t>
-  </si>
-  <si>
-    <t>Número no disponible se envia información general por mail</t>
-  </si>
-  <si>
-    <t>No dejó telefono. Se le envió mail de presentación. Seguimiento por mail.</t>
-  </si>
-  <si>
-    <t>Entra buzón, se leenió mail de presentación. Seguimiento</t>
-  </si>
-  <si>
-    <t>El teléfono está incorrecto, se le envía información general de 2 y 3 recamaras por mail.</t>
-  </si>
-  <si>
-    <t>No contesta. Mail de presentación.
-Seguimiento</t>
-  </si>
-  <si>
-    <t>Solicita información de departamentos de 3 recamaras se envia por whats</t>
-  </si>
-  <si>
-    <t>No dejó teléfono, se le envía mail de presentación.
-Seguimiento</t>
-  </si>
-  <si>
-    <t>Solicitó información de departamentos de 2 recámaras, información enviada por whats</t>
-  </si>
-  <si>
-    <t>Busca de tres recamaras y me dice que tiene $3m. pero que de cualquier forma le envíe la cotización del 205B</t>
-  </si>
-  <si>
-    <t>06 - 12 de Abril del 2020</t>
-  </si>
-  <si>
-    <t>Se envía presentación digital y cotización del 205B</t>
-  </si>
-  <si>
-    <t>No deja teléfono se envía información por mail</t>
+    <t>Se le envía información de 2 recamaras por whats</t>
+  </si>
+  <si>
+    <t>Entra buzón a la primera, se le envió mail de presentación y cotizaciones de 2 y 3 recamaras.</t>
+  </si>
+  <si>
+    <t>Me colgó a mitad de la llamada.</t>
+  </si>
+  <si>
+    <t>El telefono que dejo solo cuenta con servicio para navegar en internet  5513841692, se envia informacion por mail</t>
+  </si>
+  <si>
+    <t>No dejo teléfono, se le envió mail de presentación y cotización de 2 y 3 recamaras.</t>
+  </si>
+  <si>
+    <t>Se le envía información general por whats de 2 y 3 recamaras</t>
+  </si>
+  <si>
+    <t>Quieren vender su casa en los Cabos y venirse a vivir a México se le envió información de 2 y 3 recamaras por whats.</t>
+  </si>
+  <si>
+    <t>Llamada Whatsapp. Se le envía información de 2 y de 3 recamaras.</t>
+  </si>
+  <si>
+    <t>Llamada Whatsapp. 
+Solicita información, por whatsapp departamento 307A.</t>
+  </si>
+  <si>
+    <t>No lo gro comunicarme, se le envió mail de presentación y cotizaciones de 2 y 3 recamaras.</t>
+  </si>
+  <si>
+    <t>13 - 19 de Abril del 2020</t>
+  </si>
+  <si>
+    <t>No contesta, Se le envía información general por whats y por mail</t>
+  </si>
+  <si>
+    <t>Se le envia información por whatsapp departamentos de 3 recamaras.</t>
+  </si>
+  <si>
+    <t>Se le envía brochure digital e información general por mail</t>
+  </si>
+  <si>
+    <t>Andres Michel Rodrígez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ana cristina martinez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martini </t>
   </si>
 </sst>
 </file>
@@ -1054,13 +950,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1054100</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1257300</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>203258</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1398,10 +1294,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A4:L261"/>
+  <dimension ref="A4:L253"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1457,7 +1353,7 @@
     </row>
     <row r="16" spans="2:10" ht="23" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
-        <v>223</v>
+        <v>185</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="8"/>
@@ -1492,7 +1388,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="34">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E20" s="33" t="s">
         <v>21</v>
@@ -1511,7 +1407,7 @@
         <v>22</v>
       </c>
       <c r="F21" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="31"/>
@@ -1524,7 +1420,7 @@
         <v>23</v>
       </c>
       <c r="F22" s="34">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="31"/>
@@ -1537,7 +1433,7 @@
         <v>24</v>
       </c>
       <c r="F23" s="34">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="9"/>
@@ -1557,13 +1453,13 @@
         <v>29</v>
       </c>
       <c r="C25" s="34">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E25" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="34">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="9"/>
@@ -1574,13 +1470,13 @@
         <v>30</v>
       </c>
       <c r="C26" s="34">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E26" s="33" t="s">
         <v>27</v>
       </c>
       <c r="F26" s="34">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="9"/>
@@ -1597,7 +1493,7 @@
         <v>31</v>
       </c>
       <c r="F27" s="34">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="9"/>
@@ -1622,7 +1518,7 @@
         <v>33</v>
       </c>
       <c r="F29" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="9"/>
@@ -1682,28 +1578,26 @@
         <v>1</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F34" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="G34" s="39">
-        <v>5535665869</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="G34" s="39"/>
       <c r="H34" s="39" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="I34" s="39" t="s">
-        <v>224</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.25">
@@ -1714,25 +1608,25 @@
         <v>29</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F35" s="39" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="G35" s="39">
-        <v>5545136440</v>
+        <v>5614005671</v>
       </c>
       <c r="H35" s="39" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="I35" s="39" t="s">
-        <v>189</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1740,10 +1634,10 @@
         <v>3</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D36" s="38" t="s">
         <v>3</v>
@@ -1752,16 +1646,16 @@
         <v>13</v>
       </c>
       <c r="F36" s="39" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="G36" s="39">
-        <v>4433457580</v>
+        <v>5541426527</v>
       </c>
       <c r="H36" s="39" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="I36" s="39" t="s">
-        <v>193</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1772,7 +1666,7 @@
         <v>30</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D37" s="38" t="s">
         <v>3</v>
@@ -1781,16 +1675,16 @@
         <v>13</v>
       </c>
       <c r="F37" s="39" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G37" s="39">
-        <v>5513105111</v>
+        <v>5523196455</v>
       </c>
       <c r="H37" s="39" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="I37" s="39" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1801,7 +1695,7 @@
         <v>30</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D38" s="38" t="s">
         <v>3</v>
@@ -1810,16 +1704,16 @@
         <v>13</v>
       </c>
       <c r="F38" s="39" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G38" s="39">
-        <v>5534665530</v>
+        <v>6241540611</v>
       </c>
       <c r="H38" s="39" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="I38" s="39" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1827,28 +1721,28 @@
         <v>6</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="D39" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F39" s="39" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
       <c r="G39" s="39">
-        <v>5543610396</v>
+        <v>7122247200</v>
       </c>
       <c r="H39" s="39" t="s">
-        <v>165</v>
+        <v>112</v>
       </c>
       <c r="I39" s="39" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1856,28 +1750,28 @@
         <v>7</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C40" s="39" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="D40" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E40" s="39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F40" s="39" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
       <c r="G40" s="39">
-        <v>3314178186</v>
+        <v>5512353638</v>
       </c>
       <c r="H40" s="39" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="I40" s="39" t="s">
-        <v>212</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1885,28 +1779,28 @@
         <v>8</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C41" s="39" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D41" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F41" s="39" t="s">
-        <v>127</v>
+        <v>189</v>
       </c>
       <c r="G41" s="39">
-        <v>5528532883</v>
+        <v>5536599923</v>
       </c>
       <c r="H41" s="39" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="I41" s="39" t="s">
-        <v>219</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1914,10 +1808,10 @@
         <v>9</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C42" s="39" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D42" s="38" t="s">
         <v>3</v>
@@ -1926,16 +1820,16 @@
         <v>31</v>
       </c>
       <c r="F42" s="39" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="G42" s="39">
-        <v>5578913325</v>
+        <v>5580664676</v>
       </c>
       <c r="H42" s="39" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="I42" s="39" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1943,10 +1837,10 @@
         <v>10</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D43" s="38" t="s">
         <v>3</v>
@@ -1955,16 +1849,16 @@
         <v>31</v>
       </c>
       <c r="F43" s="39" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="G43" s="39">
-        <v>5579076952</v>
+        <v>5586180506</v>
       </c>
       <c r="H43" s="39" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="I43" s="39" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1972,7 +1866,7 @@
         <v>11</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C44" s="39" t="s">
         <v>60</v>
@@ -1984,16 +1878,16 @@
         <v>31</v>
       </c>
       <c r="F44" s="39" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G44" s="39">
-        <v>5520659177</v>
+        <v>5527656800</v>
       </c>
       <c r="H44" s="39" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="I44" s="39" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2004,7 +1898,7 @@
         <v>30</v>
       </c>
       <c r="C45" s="39" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D45" s="38" t="s">
         <v>3</v>
@@ -2013,16 +1907,16 @@
         <v>31</v>
       </c>
       <c r="F45" s="39" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="G45" s="39">
-        <v>5568875495</v>
+        <v>7712196127</v>
       </c>
       <c r="H45" s="39" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="I45" s="39" t="s">
-        <v>221</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2033,7 +1927,7 @@
         <v>34</v>
       </c>
       <c r="C46" s="39" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D46" s="38" t="s">
         <v>3</v>
@@ -2042,16 +1936,16 @@
         <v>14</v>
       </c>
       <c r="F46" s="39" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G46" s="39">
-        <v>8117910498</v>
+        <v>5539334916</v>
       </c>
       <c r="H46" s="39" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="I46" s="39" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2059,10 +1953,10 @@
         <v>14</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D47" s="38" t="s">
         <v>3</v>
@@ -2071,16 +1965,16 @@
         <v>14</v>
       </c>
       <c r="F47" s="39" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="G47" s="39">
-        <v>5512888554</v>
+        <v>5534199158</v>
       </c>
       <c r="H47" s="39" t="s">
-        <v>163</v>
+        <v>123</v>
       </c>
       <c r="I47" s="39" t="s">
-        <v>207</v>
+        <v>160</v>
       </c>
       <c r="J47" s="12"/>
     </row>
@@ -2089,26 +1983,28 @@
         <v>15</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C48" s="39" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="D48" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E48" s="39" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="F48" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="G48" s="39"/>
+        <v>110</v>
+      </c>
+      <c r="G48" s="39">
+        <v>5533967102</v>
+      </c>
       <c r="H48" s="39" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="I48" s="39" t="s">
-        <v>225</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2116,28 +2012,28 @@
         <v>16</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C49" s="39" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E49" s="39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F49" s="39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G49" s="39">
-        <v>6142157084</v>
+        <v>5530350424</v>
       </c>
       <c r="H49" s="39" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="I49" s="39" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2145,28 +2041,28 @@
         <v>17</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C50" s="39" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E50" s="39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F50" s="39" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G50" s="39">
-        <v>7224158435</v>
+        <v>6413228237</v>
       </c>
       <c r="H50" s="39" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I50" s="39" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2174,28 +2070,28 @@
         <v>18</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C51" s="39" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E51" s="39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F51" s="39" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="G51" s="39">
-        <v>5519004553</v>
+        <v>5525609124</v>
       </c>
       <c r="H51" s="39" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="I51" s="39" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2206,7 +2102,7 @@
         <v>29</v>
       </c>
       <c r="C52" s="39" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D52" s="38" t="s">
         <v>5</v>
@@ -2215,16 +2111,16 @@
         <v>13</v>
       </c>
       <c r="F52" s="39" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="G52" s="39">
-        <v>5528620367</v>
+        <v>41738560</v>
       </c>
       <c r="H52" s="39" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="I52" s="39" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2235,7 +2131,7 @@
         <v>29</v>
       </c>
       <c r="C53" s="39" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D53" s="38" t="s">
         <v>5</v>
@@ -2244,16 +2140,16 @@
         <v>13</v>
       </c>
       <c r="F53" s="39" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="G53" s="39">
-        <v>5537337373</v>
+        <v>5554376496</v>
       </c>
       <c r="H53" s="39" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="I53" s="39" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2264,7 +2160,7 @@
         <v>29</v>
       </c>
       <c r="C54" s="39" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D54" s="38" t="s">
         <v>5</v>
@@ -2273,16 +2169,16 @@
         <v>13</v>
       </c>
       <c r="F54" s="39" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="G54" s="39">
-        <v>5554019873</v>
+        <v>5518471074</v>
       </c>
       <c r="H54" s="39" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="I54" s="39" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2293,7 +2189,7 @@
         <v>29</v>
       </c>
       <c r="C55" s="39" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D55" s="38" t="s">
         <v>5</v>
@@ -2302,16 +2198,14 @@
         <v>13</v>
       </c>
       <c r="F55" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="G55" s="39">
-        <v>5525611447</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="G55" s="39"/>
       <c r="H55" s="39" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="I55" s="39" t="s">
-        <v>208</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2322,7 +2216,7 @@
         <v>29</v>
       </c>
       <c r="C56" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D56" s="38" t="s">
         <v>5</v>
@@ -2331,16 +2225,16 @@
         <v>13</v>
       </c>
       <c r="F56" s="39" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="G56" s="39">
-        <v>553466554</v>
+        <v>5519515706</v>
       </c>
       <c r="H56" s="39" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="I56" s="39" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2351,7 +2245,7 @@
         <v>29</v>
       </c>
       <c r="C57" s="39" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D57" s="38" t="s">
         <v>5</v>
@@ -2360,16 +2254,16 @@
         <v>13</v>
       </c>
       <c r="F57" s="39" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="G57" s="39">
-        <v>5544487681</v>
+        <v>5523004330</v>
       </c>
       <c r="H57" s="39" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="I57" s="39" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2380,7 +2274,7 @@
         <v>29</v>
       </c>
       <c r="C58" s="39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D58" s="38" t="s">
         <v>5</v>
@@ -2389,16 +2283,16 @@
         <v>13</v>
       </c>
       <c r="F58" s="39" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="G58" s="39">
-        <v>5525590602</v>
+        <v>5569006106</v>
       </c>
       <c r="H58" s="39" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="I58" s="39" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2406,10 +2300,10 @@
         <v>26</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C59" s="39" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="D59" s="38" t="s">
         <v>5</v>
@@ -2418,16 +2312,16 @@
         <v>13</v>
       </c>
       <c r="F59" s="39" t="s">
-        <v>126</v>
+        <v>78</v>
       </c>
       <c r="G59" s="39">
-        <v>5533108080</v>
+        <v>5513335213</v>
       </c>
       <c r="H59" s="39" t="s">
-        <v>174</v>
+        <v>115</v>
       </c>
       <c r="I59" s="39" t="s">
-        <v>218</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2435,10 +2329,10 @@
         <v>27</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C60" s="39" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="D60" s="38" t="s">
         <v>5</v>
@@ -2447,16 +2341,16 @@
         <v>13</v>
       </c>
       <c r="F60" s="39" t="s">
-        <v>130</v>
+        <v>82</v>
       </c>
       <c r="G60" s="39">
-        <v>5514399159</v>
+        <v>4442013260</v>
       </c>
       <c r="H60" s="39" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="I60" s="39" t="s">
-        <v>222</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2467,7 +2361,7 @@
         <v>30</v>
       </c>
       <c r="C61" s="39" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D61" s="38" t="s">
         <v>5</v>
@@ -2476,16 +2370,16 @@
         <v>13</v>
       </c>
       <c r="F61" s="39" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G61" s="39">
-        <v>3314118246</v>
+        <v>5512965912</v>
       </c>
       <c r="H61" s="39" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I61" s="39" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2496,7 +2390,7 @@
         <v>30</v>
       </c>
       <c r="C62" s="39" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="D62" s="38" t="s">
         <v>5</v>
@@ -2505,16 +2399,16 @@
         <v>13</v>
       </c>
       <c r="F62" s="39" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="G62" s="39">
-        <v>5523945289</v>
+        <v>5548998870</v>
       </c>
       <c r="H62" s="39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I62" s="39" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2522,28 +2416,28 @@
         <v>30</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C63" s="39" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D63" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E63" s="39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F63" s="39" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G63" s="39">
-        <v>5547831625</v>
+        <v>5516821634</v>
       </c>
       <c r="H63" s="39" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="I63" s="39" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2551,28 +2445,28 @@
         <v>31</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C64" s="39" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D64" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E64" s="39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F64" s="39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G64" s="39">
-        <v>5527379917</v>
+        <v>7225336736</v>
       </c>
       <c r="H64" s="39" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="I64" s="39" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2580,28 +2474,28 @@
         <v>32</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C65" s="39" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D65" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F65" s="39" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G65" s="39">
-        <v>5549403963</v>
+        <v>6624717691</v>
       </c>
       <c r="H65" s="39" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="I65" s="39" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2609,28 +2503,28 @@
         <v>33</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C66" s="39" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D66" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E66" s="39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F66" s="39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G66" s="39">
-        <v>984567890</v>
+        <v>4499119282</v>
       </c>
       <c r="H66" s="39" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="I66" s="39" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2638,28 +2532,26 @@
         <v>34</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C67" s="39" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D67" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E67" s="39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F67" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="G67" s="39">
-        <v>5520807149</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="G67" s="39"/>
       <c r="H67" s="39" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="I67" s="39" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2667,7 +2559,7 @@
         <v>35</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C68" s="39" t="s">
         <v>74</v>
@@ -2676,19 +2568,19 @@
         <v>5</v>
       </c>
       <c r="E68" s="39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F68" s="39" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G68" s="39">
-        <v>5534330708</v>
+        <v>5538853148</v>
       </c>
       <c r="H68" s="39" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="I68" s="39" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="17" x14ac:dyDescent="0.25">
@@ -2699,25 +2591,25 @@
         <v>30</v>
       </c>
       <c r="C69" s="39" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="D69" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E69" s="39" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="F69" s="39" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="G69" s="39">
-        <v>5549406742</v>
+        <v>5564150057</v>
       </c>
       <c r="H69" s="39" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="I69" s="39" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="17" x14ac:dyDescent="0.25">
@@ -2725,10 +2617,10 @@
         <v>37</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C70" s="39" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D70" s="38" t="s">
         <v>5</v>
@@ -2737,16 +2629,16 @@
         <v>31</v>
       </c>
       <c r="F70" s="39" t="s">
-        <v>86</v>
+        <v>190</v>
       </c>
       <c r="G70" s="39">
-        <v>6682302763</v>
+        <v>5560707606</v>
       </c>
       <c r="H70" s="39" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I70" s="39" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="17" x14ac:dyDescent="0.25">
@@ -2754,10 +2646,10 @@
         <v>38</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C71" s="39" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D71" s="38" t="s">
         <v>5</v>
@@ -2766,16 +2658,16 @@
         <v>31</v>
       </c>
       <c r="F71" s="39" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="G71" s="39">
-        <v>9933839643</v>
+        <v>5579243781</v>
       </c>
       <c r="H71" s="39" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="I71" s="39" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="17" x14ac:dyDescent="0.25">
@@ -2783,10 +2675,10 @@
         <v>39</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C72" s="39" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D72" s="38" t="s">
         <v>5</v>
@@ -2795,16 +2687,16 @@
         <v>31</v>
       </c>
       <c r="F72" s="39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G72" s="39">
-        <v>5528369143</v>
+        <v>9512338043</v>
       </c>
       <c r="H72" s="39" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="I72" s="39" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="17" x14ac:dyDescent="0.25">
@@ -2812,10 +2704,10 @@
         <v>40</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C73" s="39" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D73" s="38" t="s">
         <v>5</v>
@@ -2824,355 +2716,208 @@
         <v>31</v>
       </c>
       <c r="F73" s="39" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G73" s="39">
-        <v>4772740950</v>
+        <v>13841692</v>
       </c>
       <c r="H73" s="39" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="I73" s="39" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>41</v>
-      </c>
-      <c r="B74" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C74" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D74" s="38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="11" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="39"/>
+      <c r="C74" s="40"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="41"/>
+      <c r="H74" s="42"/>
+      <c r="I74" s="41"/>
+    </row>
+    <row r="75" spans="1:9" ht="11" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="39"/>
+      <c r="C75" s="40"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="38"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="41"/>
+      <c r="H75" s="42"/>
+      <c r="I75" s="41"/>
+    </row>
+    <row r="76" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" s="19"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="20"/>
+      <c r="I76" s="12"/>
+    </row>
+    <row r="77" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="18"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="20"/>
+      <c r="I77" s="12"/>
+    </row>
+    <row r="78" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="18"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="20"/>
+      <c r="I78" s="12"/>
+    </row>
+    <row r="79" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C79" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79" s="24"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="26"/>
+      <c r="G79" s="27"/>
+      <c r="H79" s="28"/>
+      <c r="I79" s="12"/>
+    </row>
+    <row r="80" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C80" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D80" s="24"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="26"/>
+      <c r="G80" s="27"/>
+      <c r="H80" s="28"/>
+      <c r="I80" s="12"/>
+    </row>
+    <row r="81" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="24"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="26"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="28"/>
+      <c r="I81" s="12"/>
+    </row>
+    <row r="82" spans="2:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="B82" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E74" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F74" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="G74" s="39"/>
-      <c r="H74" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="I74" s="39" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>42</v>
-      </c>
-      <c r="B75" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C75" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="D75" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E75" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F75" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="G75" s="39">
-        <v>9982607326</v>
-      </c>
-      <c r="H75" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="I75" s="39" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>43</v>
-      </c>
-      <c r="B76" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C76" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="D76" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E76" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F76" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="G76" s="39"/>
-      <c r="H76" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="I76" s="39" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
-        <v>44</v>
-      </c>
-      <c r="B77" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C77" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D77" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E77" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F77" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="G77" s="39">
-        <v>5525115818</v>
-      </c>
-      <c r="H77" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="I77" s="39" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>45</v>
-      </c>
-      <c r="B78" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C78" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="D78" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E78" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F78" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="G78" s="39">
-        <v>5526845542</v>
-      </c>
-      <c r="H78" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="I78" s="39" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>46</v>
-      </c>
-      <c r="B79" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C79" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="D79" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E79" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F79" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="G79" s="39">
-        <v>6647427716</v>
-      </c>
-      <c r="H79" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="I79" s="39" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
-        <v>47</v>
-      </c>
-      <c r="B80" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C80" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="D80" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E80" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F80" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="G80" s="39">
-        <v>5521359499</v>
-      </c>
-      <c r="H80" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="I80" s="39" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>48</v>
-      </c>
-      <c r="B81" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C81" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="D81" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E81" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F81" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="G81" s="39">
-        <v>5543374357</v>
-      </c>
-      <c r="H81" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="I81" s="39" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="11" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="39"/>
-      <c r="C82" s="40"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="38"/>
-      <c r="F82" s="38"/>
-      <c r="G82" s="41"/>
-      <c r="H82" s="42"/>
-      <c r="I82" s="41"/>
-    </row>
-    <row r="83" spans="1:10" ht="11" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="39"/>
-      <c r="C83" s="40"/>
-      <c r="D83" s="38"/>
-      <c r="E83" s="38"/>
-      <c r="F83" s="38"/>
-      <c r="G83" s="41"/>
-      <c r="H83" s="42"/>
-      <c r="I83" s="41"/>
-    </row>
-    <row r="84" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C84" s="19"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="20"/>
-      <c r="I84" s="12"/>
-    </row>
-    <row r="85" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="18"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="18"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="20"/>
-      <c r="I85" s="12"/>
-    </row>
-    <row r="86" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="18"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="18"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="18"/>
-      <c r="G86" s="12"/>
-      <c r="H86" s="20"/>
-      <c r="I86" s="12"/>
-    </row>
-    <row r="87" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C87" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D87" s="24"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="26"/>
-      <c r="G87" s="27"/>
-      <c r="H87" s="28"/>
-      <c r="I87" s="12"/>
-    </row>
-    <row r="88" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C88" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D88" s="24"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="26"/>
-      <c r="G88" s="27"/>
-      <c r="H88" s="28"/>
-      <c r="I88" s="12"/>
-    </row>
-    <row r="89" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C89" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D89" s="24"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="26"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="28"/>
-      <c r="I89" s="12"/>
-    </row>
-    <row r="90" spans="1:10" ht="17" x14ac:dyDescent="0.25">
-      <c r="B90" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="23" t="s">
+      <c r="C82" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D90" s="24"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="29"/>
-      <c r="H90" s="30"/>
-      <c r="I90" s="6"/>
-    </row>
-    <row r="91" spans="1:10" ht="16" x14ac:dyDescent="0.25">
+      <c r="D82" s="24"/>
+      <c r="E82" s="25"/>
+      <c r="F82" s="25"/>
+      <c r="G82" s="29"/>
+      <c r="H82" s="30"/>
+      <c r="I82" s="6"/>
+    </row>
+    <row r="83" spans="2:12" ht="16" x14ac:dyDescent="0.25">
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="6"/>
+      <c r="I83" s="6"/>
+    </row>
+    <row r="84" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="6"/>
+      <c r="I84" s="6"/>
+    </row>
+    <row r="85" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="21"/>
+    </row>
+    <row r="86" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="21"/>
+    </row>
+    <row r="87" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="21"/>
+    </row>
+    <row r="88" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="21"/>
+    </row>
+    <row r="89" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="21"/>
+    </row>
+    <row r="90" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="21"/>
+    </row>
+    <row r="91" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
@@ -3180,8 +2925,9 @@
       <c r="F91" s="5"/>
       <c r="G91" s="6"/>
       <c r="I91" s="6"/>
-    </row>
-    <row r="92" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J91" s="21"/>
+    </row>
+    <row r="92" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
@@ -3189,8 +2935,9 @@
       <c r="F92" s="5"/>
       <c r="G92" s="6"/>
       <c r="I92" s="6"/>
-    </row>
-    <row r="93" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J92" s="21"/>
+    </row>
+    <row r="93" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
@@ -3198,9 +2945,11 @@
       <c r="F93" s="5"/>
       <c r="G93" s="6"/>
       <c r="I93" s="6"/>
-      <c r="J93" s="21"/>
-    </row>
-    <row r="94" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+    </row>
+    <row r="94" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
@@ -3208,9 +2957,11 @@
       <c r="F94" s="5"/>
       <c r="G94" s="6"/>
       <c r="I94" s="6"/>
-      <c r="J94" s="21"/>
-    </row>
-    <row r="95" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
+    </row>
+    <row r="95" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
@@ -3218,19 +2969,21 @@
       <c r="F95" s="5"/>
       <c r="G95" s="6"/>
       <c r="I95" s="6"/>
-      <c r="J95" s="21"/>
-    </row>
-    <row r="96" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="6"/>
+    </row>
+    <row r="96" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="6"/>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
       <c r="E96" s="6"/>
       <c r="F96" s="5"/>
       <c r="G96" s="6"/>
       <c r="I96" s="6"/>
-      <c r="J96" s="21"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
     </row>
     <row r="97" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="6"/>
@@ -3240,18 +2993,21 @@
       <c r="F97" s="5"/>
       <c r="G97" s="6"/>
       <c r="I97" s="6"/>
-      <c r="J97" s="21"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="6"/>
     </row>
     <row r="98" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
-      <c r="G98" s="3"/>
-      <c r="H98" s="4"/>
-      <c r="I98" s="3"/>
-      <c r="J98" s="21"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="6"/>
     </row>
     <row r="99" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="6"/>
@@ -3261,7 +3017,9 @@
       <c r="F99" s="5"/>
       <c r="G99" s="6"/>
       <c r="I99" s="6"/>
-      <c r="J99" s="21"/>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="6"/>
     </row>
     <row r="100" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="6"/>
@@ -3271,7 +3029,9 @@
       <c r="F100" s="5"/>
       <c r="G100" s="6"/>
       <c r="I100" s="6"/>
-      <c r="J100" s="21"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="6"/>
     </row>
     <row r="101" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="6"/>
@@ -3281,7 +3041,7 @@
       <c r="F101" s="5"/>
       <c r="G101" s="6"/>
       <c r="I101" s="6"/>
-      <c r="J101" s="6"/>
+      <c r="J101" s="3"/>
       <c r="K101" s="6"/>
       <c r="L101" s="6"/>
     </row>
@@ -3377,7 +3137,7 @@
       <c r="F109" s="5"/>
       <c r="G109" s="6"/>
       <c r="I109" s="6"/>
-      <c r="J109" s="3"/>
+      <c r="J109" s="6"/>
       <c r="K109" s="6"/>
       <c r="L109" s="6"/>
     </row>
@@ -4978,97 +4738,41 @@
       <c r="L242" s="6"/>
     </row>
     <row r="243" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B243" s="6"/>
-      <c r="C243" s="6"/>
-      <c r="D243" s="6"/>
-      <c r="E243" s="6"/>
-      <c r="F243" s="5"/>
-      <c r="G243" s="6"/>
-      <c r="I243" s="6"/>
       <c r="J243" s="6"/>
       <c r="K243" s="6"/>
       <c r="L243" s="6"/>
     </row>
     <row r="244" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B244" s="6"/>
-      <c r="C244" s="6"/>
-      <c r="D244" s="6"/>
-      <c r="E244" s="6"/>
-      <c r="F244" s="5"/>
-      <c r="G244" s="6"/>
-      <c r="I244" s="6"/>
       <c r="J244" s="6"/>
       <c r="K244" s="6"/>
       <c r="L244" s="6"/>
     </row>
     <row r="245" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B245" s="6"/>
-      <c r="C245" s="6"/>
-      <c r="D245" s="6"/>
-      <c r="E245" s="6"/>
-      <c r="F245" s="5"/>
-      <c r="G245" s="6"/>
-      <c r="I245" s="6"/>
       <c r="J245" s="6"/>
       <c r="K245" s="6"/>
       <c r="L245" s="6"/>
     </row>
     <row r="246" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B246" s="6"/>
-      <c r="C246" s="6"/>
-      <c r="D246" s="6"/>
-      <c r="E246" s="6"/>
-      <c r="F246" s="5"/>
-      <c r="G246" s="6"/>
-      <c r="I246" s="6"/>
       <c r="J246" s="6"/>
       <c r="K246" s="6"/>
       <c r="L246" s="6"/>
     </row>
     <row r="247" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B247" s="6"/>
-      <c r="C247" s="6"/>
-      <c r="D247" s="6"/>
-      <c r="E247" s="6"/>
-      <c r="F247" s="5"/>
-      <c r="G247" s="6"/>
-      <c r="I247" s="6"/>
       <c r="J247" s="6"/>
       <c r="K247" s="6"/>
       <c r="L247" s="6"/>
     </row>
     <row r="248" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B248" s="6"/>
-      <c r="C248" s="6"/>
-      <c r="D248" s="6"/>
-      <c r="E248" s="6"/>
-      <c r="F248" s="5"/>
-      <c r="G248" s="6"/>
-      <c r="I248" s="6"/>
       <c r="J248" s="6"/>
       <c r="K248" s="6"/>
       <c r="L248" s="6"/>
     </row>
     <row r="249" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B249" s="6"/>
-      <c r="C249" s="6"/>
-      <c r="D249" s="6"/>
-      <c r="E249" s="6"/>
-      <c r="F249" s="5"/>
-      <c r="G249" s="6"/>
-      <c r="I249" s="6"/>
       <c r="J249" s="6"/>
       <c r="K249" s="6"/>
       <c r="L249" s="6"/>
     </row>
     <row r="250" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B250" s="6"/>
-      <c r="C250" s="6"/>
-      <c r="D250" s="6"/>
-      <c r="E250" s="6"/>
-      <c r="F250" s="5"/>
-      <c r="G250" s="6"/>
-      <c r="I250" s="6"/>
       <c r="J250" s="6"/>
       <c r="K250" s="6"/>
       <c r="L250" s="6"/>
@@ -5088,48 +4792,8 @@
       <c r="K253" s="6"/>
       <c r="L253" s="6"/>
     </row>
-    <row r="254" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J254" s="6"/>
-      <c r="K254" s="6"/>
-      <c r="L254" s="6"/>
-    </row>
-    <row r="255" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J255" s="6"/>
-      <c r="K255" s="6"/>
-      <c r="L255" s="6"/>
-    </row>
-    <row r="256" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J256" s="6"/>
-      <c r="K256" s="6"/>
-      <c r="L256" s="6"/>
-    </row>
-    <row r="257" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J257" s="6"/>
-      <c r="K257" s="6"/>
-      <c r="L257" s="6"/>
-    </row>
-    <row r="258" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J258" s="6"/>
-      <c r="K258" s="6"/>
-      <c r="L258" s="6"/>
-    </row>
-    <row r="259" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J259" s="6"/>
-      <c r="K259" s="6"/>
-      <c r="L259" s="6"/>
-    </row>
-    <row r="260" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J260" s="6"/>
-      <c r="K260" s="6"/>
-      <c r="L260" s="6"/>
-    </row>
-    <row r="261" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J261" s="6"/>
-      <c r="K261" s="6"/>
-      <c r="L261" s="6"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:A81">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:A73">
     <sortCondition ref="A34"/>
   </sortState>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
19 to 24 of April report
</commit_message>
<xml_diff>
--- a/public/reports/Reporte_Avenue_Napoles.xlsx
+++ b/public/reports/Reporte_Avenue_Napoles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergirams/Development/Kiper/backend/apikiper/public/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF26C910-87D1-104D-9351-4A9276728217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41B3E1BA-C945-0F4B-A97D-874C2E14824A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27480" yWindow="460" windowWidth="34720" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25880" yWindow="520" windowWidth="37880" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="183">
   <si>
     <t>A</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Facebook</t>
   </si>
   <si>
-    <t>Manual</t>
-  </si>
-  <si>
     <t>Reporte Oficina de Ventas</t>
   </si>
   <si>
@@ -134,487 +131,466 @@
     <t>Messenger</t>
   </si>
   <si>
-    <t>Alejandra Campos García</t>
-  </si>
-  <si>
-    <t>2020-04-19 17:33:40</t>
-  </si>
-  <si>
-    <t>2020-04-19 17:09:05</t>
-  </si>
-  <si>
-    <t>2020-04-19 13:20:42</t>
-  </si>
-  <si>
-    <t>2020-04-19 11:43:05</t>
-  </si>
-  <si>
-    <t>2020-04-19 01:21:04</t>
-  </si>
-  <si>
-    <t>2020-04-18 18:56:18</t>
-  </si>
-  <si>
-    <t>2020-04-18 11:54:19</t>
-  </si>
-  <si>
-    <t>2020-04-18 11:22:06</t>
-  </si>
-  <si>
-    <t>2020-04-18 00:37:06</t>
-  </si>
-  <si>
-    <t>2020-04-17 22:11:30</t>
-  </si>
-  <si>
-    <t>2020-04-17 20:28:21</t>
-  </si>
-  <si>
-    <t>2020-04-17 15:08:09</t>
-  </si>
-  <si>
-    <t>2020-04-17 10:11:25</t>
-  </si>
-  <si>
-    <t>2020-04-16 23:47:54</t>
-  </si>
-  <si>
-    <t>2020-04-16 21:59:41</t>
-  </si>
-  <si>
-    <t>2020-04-16 19:20:49</t>
-  </si>
-  <si>
-    <t>2020-04-16 13:41:50</t>
-  </si>
-  <si>
-    <t>2020-04-15 22:34:38</t>
-  </si>
-  <si>
-    <t>2020-04-15 21:54:44</t>
-  </si>
-  <si>
-    <t>2020-04-15 17:48:40</t>
-  </si>
-  <si>
-    <t>2020-04-15 14:29:39</t>
-  </si>
-  <si>
-    <t>2020-04-15 07:40:48</t>
-  </si>
-  <si>
-    <t>2020-04-15 00:21:10</t>
-  </si>
-  <si>
-    <t>2020-04-14 22:47:19</t>
-  </si>
-  <si>
-    <t>2020-04-14 22:32:59</t>
-  </si>
-  <si>
-    <t>2020-04-14 17:18:17</t>
-  </si>
-  <si>
-    <t>2020-04-14 12:53:15</t>
-  </si>
-  <si>
-    <t>2020-04-14 12:38:17</t>
-  </si>
-  <si>
-    <t>2020-04-14 08:02:26</t>
-  </si>
-  <si>
-    <t>2020-04-14 07:12:10</t>
-  </si>
-  <si>
-    <t>2020-04-14 01:39:59</t>
-  </si>
-  <si>
-    <t>2020-04-13 23:58:11</t>
-  </si>
-  <si>
-    <t>2020-04-13 22:41:25</t>
-  </si>
-  <si>
-    <t>2020-04-13 19:38:20</t>
-  </si>
-  <si>
-    <t>2020-04-13 16:00:41</t>
-  </si>
-  <si>
-    <t>2020-04-13 15:34:29</t>
-  </si>
-  <si>
-    <t>2020-04-13 14:45:34</t>
-  </si>
-  <si>
-    <t>2020-04-13 13:00:02</t>
-  </si>
-  <si>
-    <t>2020-04-13 12:55:29</t>
-  </si>
-  <si>
-    <t>2020-04-13 11:35:15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lizbeth Becerril Contreras </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alicia Gtz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerardo Marin </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melissa Alvarez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nuria Yunuen </t>
-  </si>
-  <si>
-    <t>Edgar Salas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carmina Rodriguez Zaldivar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ilse Nayeli </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Midori abigail silva Reyes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tania Annirack Flores García </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mafalda Comales </t>
-  </si>
-  <si>
-    <t>Elizabeth Gonzalez</t>
-  </si>
-  <si>
-    <t>Diana Aline Garcia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yuri Sevilla </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samantha Shs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jose Fragoso </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brayan Valdes Vazquez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diego Trujillo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alejandro Rivera centeno </t>
-  </si>
-  <si>
-    <t>Jesus Andres Garcia Medina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roberto Gonzalez Labastida </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marco </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adriana Islas Romero </t>
-  </si>
-  <si>
-    <t xml:space="preserve">María Esmeralda Lopez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ana Aguirre </t>
-  </si>
-  <si>
-    <t>Luis Gonzalez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Garbu </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alan Amador Perez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guadalupe Cárdenas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">marco antonio Ramírez Ortiz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elizabeth </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atlantida Resendiz Cruz </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grace Izquierdo Molleda </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noel Acosta </t>
-  </si>
-  <si>
-    <t>Mariana Ituarte</t>
-  </si>
-  <si>
-    <t>Manuel Dovali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jennifer </t>
-  </si>
-  <si>
-    <t>lbecerril018@gmail.com</t>
-  </si>
-  <si>
-    <t>alizzgo_78@hotmail.com</t>
-  </si>
-  <si>
-    <t>gmarin2000@hotmail.com</t>
-  </si>
-  <si>
-    <t>Mel-alvarez@hotmail.com</t>
-  </si>
-  <si>
-    <t>nuria_y_om@icloud.com</t>
-  </si>
-  <si>
-    <t>edgar_salas@hotmail.com</t>
-  </si>
-  <si>
-    <t>crodriguezzsldivar@gmail.com</t>
-  </si>
-  <si>
-    <t>ilse3571@hotmail.com</t>
-  </si>
-  <si>
-    <t>silvamidori986@gmail.com</t>
-  </si>
-  <si>
-    <t>maradan.tr@gmail.com</t>
-  </si>
-  <si>
-    <t>Pilrcr@hotmail.com</t>
-  </si>
-  <si>
-    <t>elypope200879@gmail.com</t>
-  </si>
-  <si>
-    <t>alinearteaga@me.com</t>
-  </si>
-  <si>
-    <t>yurisevilla@hotmail.com</t>
-  </si>
-  <si>
-    <t>shsondersam90@hotmail.com</t>
-  </si>
-  <si>
-    <t>Jofrago1302@gmail.com</t>
-  </si>
-  <si>
-    <t>valdesvzquezbrayan@gmail.com</t>
-  </si>
-  <si>
-    <t>dtrujillovaz@gmail.com</t>
-  </si>
-  <si>
-    <t>alejandro_1508@outlook.com</t>
-  </si>
-  <si>
-    <t>acmituarte@yahoo.com.mx</t>
-  </si>
-  <si>
-    <t>jesus_andres_14@hotmail.com</t>
-  </si>
-  <si>
-    <t>rogola66@live.com.mx</t>
-  </si>
-  <si>
-    <t>marcoar.galan@gmail.com</t>
-  </si>
-  <si>
-    <t>adry.islas@hotmail.com</t>
-  </si>
-  <si>
-    <t>mariaesmerald@yahoo.com</t>
-  </si>
-  <si>
-    <t>ann1323.aa@gmail.com</t>
-  </si>
-  <si>
-    <t>5539334916@phonecall.com</t>
-  </si>
-  <si>
-    <t>garbiecheverria4@gmail.com</t>
-  </si>
-  <si>
-    <t>andres.michelr@gmail.com</t>
-  </si>
-  <si>
-    <t>alanamador7@gmail.com</t>
-  </si>
-  <si>
-    <t>lucardenasgtz@gmail.com</t>
-  </si>
-  <si>
-    <t>marckram9@gmail.com</t>
-  </si>
-  <si>
-    <t>Wvc8s7SPa@outlook.com</t>
-  </si>
-  <si>
-    <t>martinidasa@yahoo.com</t>
-  </si>
-  <si>
-    <t>atlantida.resendiz@gmail.com</t>
-  </si>
-  <si>
-    <t>molledag@hotmail.com</t>
-  </si>
-  <si>
-    <t>noel.acosta17@gmail.com</t>
-  </si>
-  <si>
-    <t>ituartemariana@gmail.com</t>
-  </si>
-  <si>
-    <t>manuel.dovali@gmail.com</t>
-  </si>
-  <si>
-    <t>Jennygaray14102000@gmail.com</t>
-  </si>
-  <si>
-    <t>No contesta, se le envió mail de presentación y cotizaciones de departamentos de 2 y 3 recamaras.
-SEguimiento</t>
-  </si>
-  <si>
-    <t>No contesta telefono se le envía información general por mail</t>
-  </si>
-  <si>
-    <t>Le llamé y me dice que primero le envíe la información del proyecto y cotización de 2 y 3 recamara para que los revise.
+    <t>2020-04-26 17:14:44</t>
+  </si>
+  <si>
+    <t>2020-04-26 16:11:49</t>
+  </si>
+  <si>
+    <t>2020-04-26 14:39:49</t>
+  </si>
+  <si>
+    <t>2020-04-26 12:40:50</t>
+  </si>
+  <si>
+    <t>2020-04-26 11:50:49</t>
+  </si>
+  <si>
+    <t>2020-04-26 11:17:02</t>
+  </si>
+  <si>
+    <t>2020-04-26 00:26:05</t>
+  </si>
+  <si>
+    <t>2020-04-25 23:29:59</t>
+  </si>
+  <si>
+    <t>2020-04-25 23:20:57</t>
+  </si>
+  <si>
+    <t>2020-04-25 22:04:33</t>
+  </si>
+  <si>
+    <t>2020-04-25 21:26:16</t>
+  </si>
+  <si>
+    <t>2020-04-25 20:40:08</t>
+  </si>
+  <si>
+    <t>2020-04-25 19:11:41</t>
+  </si>
+  <si>
+    <t>2020-04-25 17:05:21</t>
+  </si>
+  <si>
+    <t>2020-04-25 13:14:39</t>
+  </si>
+  <si>
+    <t>2020-04-24 00:04:40</t>
+  </si>
+  <si>
+    <t>2020-04-23 20:31:15</t>
+  </si>
+  <si>
+    <t>2020-04-23 16:34:11</t>
+  </si>
+  <si>
+    <t>2020-04-23 16:22:04</t>
+  </si>
+  <si>
+    <t>2020-04-23 15:07:32</t>
+  </si>
+  <si>
+    <t>2020-04-23 13:02:00</t>
+  </si>
+  <si>
+    <t>2020-04-23 09:31:20</t>
+  </si>
+  <si>
+    <t>2020-04-23 01:23:58</t>
+  </si>
+  <si>
+    <t>2020-04-23 00:18:59</t>
+  </si>
+  <si>
+    <t>2020-04-22 21:09:02</t>
+  </si>
+  <si>
+    <t>2020-04-22 18:06:47</t>
+  </si>
+  <si>
+    <t>2020-04-22 14:33:53</t>
+  </si>
+  <si>
+    <t>2020-04-22 10:23:44</t>
+  </si>
+  <si>
+    <t>2020-04-21 21:02:23</t>
+  </si>
+  <si>
+    <t>2020-04-21 19:56:04</t>
+  </si>
+  <si>
+    <t>2020-04-21 15:16:25</t>
+  </si>
+  <si>
+    <t>2020-04-21 00:21:46</t>
+  </si>
+  <si>
+    <t>2020-04-20 18:56:39</t>
+  </si>
+  <si>
+    <t>2020-04-20 18:45:54</t>
+  </si>
+  <si>
+    <t>2020-04-20 18:32:46</t>
+  </si>
+  <si>
+    <t>2020-04-20 13:31:43</t>
+  </si>
+  <si>
+    <t>2020-04-20 13:22:31</t>
+  </si>
+  <si>
+    <t>2020-04-20 00:29:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rocio Fernandez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ale Adam </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estephanya melendez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gustavo aaron mendoza Garcia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haydée Calderon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arturo Alonso </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fernanda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rodolfo Espinosa De Los Monteros </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montserrat Desentis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jorgelina Figueroa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denisse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patricia del Rosal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minka Luque </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ariadna Paulina Sandoval Marín </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro Alberto Campos Benitez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Gaytan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lili5585329803 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adriana Zenteno </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dario Scherer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">juan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patricia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesus Elizondo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amelia Walker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enrique </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javier cedeño </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evelyn Kassandra Valverde Gomez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felipe Jimenez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">María Eugenia Salgado Guzman </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adriana Sampaio (broker Alur Bienes Raices) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martinez Isabel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renatta Chavez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christian Arjan Rivas Guzmán </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juana Solis Hernandez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mallorca Karol </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monica Del Rio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anaid López Martínez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axel Zamudio </t>
+  </si>
+  <si>
+    <t>rocio_fernandez_sobero@hotmail.com</t>
+  </si>
+  <si>
+    <t>aleadam@live.com.mx</t>
+  </si>
+  <si>
+    <t>paigestacyh@gmail.com</t>
+  </si>
+  <si>
+    <t>gustavoaaronmendozagarcia@gmail.com</t>
+  </si>
+  <si>
+    <t>aidecalderon18@hotmail.com</t>
+  </si>
+  <si>
+    <t>aeta_abogados@outlook.com</t>
+  </si>
+  <si>
+    <t>calisteniaystreetworkout99@gma.com</t>
+  </si>
+  <si>
+    <t>respinosan@icloud.com</t>
+  </si>
+  <si>
+    <t>montse_27@hotmail.com</t>
+  </si>
+  <si>
+    <t>jorgelina_figueroa@hotmail.com</t>
+  </si>
+  <si>
+    <t>beciezdenise260617@gmail.com</t>
+  </si>
+  <si>
+    <t>patt_me@hotmail.com</t>
+  </si>
+  <si>
+    <t>minka.luque999.9@gmail.com</t>
+  </si>
+  <si>
+    <t>ariadnamarin210102@gmail.com</t>
+  </si>
+  <si>
+    <t>pedro_benitez77@hotmail.com</t>
+  </si>
+  <si>
+    <t>David.gaytan.f@gmail.com</t>
+  </si>
+  <si>
+    <t>liliaespinisa24@yahoo.com.mx</t>
+  </si>
+  <si>
+    <t>Adriana.zenteno.rizo@gmail.com</t>
+  </si>
+  <si>
+    <t>darioschererc@gmail.com</t>
+  </si>
+  <si>
+    <t>anarodaco65@gmail.com</t>
+  </si>
+  <si>
+    <t>psierra53@icloud.com</t>
+  </si>
+  <si>
+    <t>jesus.elizondon@gmail.com</t>
+  </si>
+  <si>
+    <t>amelia1996@gmail.com</t>
+  </si>
+  <si>
+    <t>erubio811@gmail.com</t>
+  </si>
+  <si>
+    <t>obregon.6913@gmail.com</t>
+  </si>
+  <si>
+    <t>kassandravalverde7@gmail.com</t>
+  </si>
+  <si>
+    <t>fjajm@hotmail.com</t>
+  </si>
+  <si>
+    <t>maeugeny09@gmail.com</t>
+  </si>
+  <si>
+    <t>adriana@alur.mx</t>
+  </si>
+  <si>
+    <t>Isabel@c21fortaleza.com</t>
+  </si>
+  <si>
+    <t>renattavchavez@gmail.com</t>
+  </si>
+  <si>
+    <t>arjanrivas.sm@gmail.com</t>
+  </si>
+  <si>
+    <t>jsoldeoro5@gmail.com</t>
+  </si>
+  <si>
+    <t>mallor10@gmail.com</t>
+  </si>
+  <si>
+    <t>monicapdelrioc@hotmail.com</t>
+  </si>
+  <si>
+    <t>comprador@live.com.mx</t>
+  </si>
+  <si>
+    <t>anaid131193@outlook.com</t>
+  </si>
+  <si>
+    <t>axelcooper@gmail.com</t>
+  </si>
+  <si>
+    <t>No contesta se le envía información de 2 y 3 recamaras por mail</t>
+  </si>
+  <si>
+    <t>Se le envía información de 2 recamaras mas estudio</t>
+  </si>
+  <si>
+    <t>Se le envía información general por mail.</t>
+  </si>
+  <si>
+    <t>No contesta, entra buzón. Se le envió mail de presentación y cotización de 2 y 3 recamaras.
 Seguimiento</t>
   </si>
   <si>
-    <t>Visita al Showroom el sábado de 18 de Abril, se llevo información del 307A Llamarle el lunes 20</t>
-  </si>
-  <si>
-    <t>No contesta, entra buzón. se le envió mail de presentación y cotizaciones de departamentos de 2 y 3 recamaras.
+    <t>Se le envia información general por mail</t>
+  </si>
+  <si>
+    <t>Solicitó informes de 2 y 3 recamaras se le envió el 205B 
 Seguimiento</t>
   </si>
   <si>
-    <t>Entra buzón se le envía información general por mail.</t>
-  </si>
-  <si>
-    <t>Busca 2 recamaras y tiene hasta $7 millones. Se le envió cotización del 205B
+    <t>No deja teléfono se le envía información general por mail.</t>
+  </si>
+  <si>
+    <t>No contesta, se le envió mail de presentación y cotizaciones.
 Seguimiento</t>
   </si>
   <si>
-    <t>Se le envía información de 3 recamaras por whats y Tiene cita programada para el Jueves 23 de Abril</t>
-  </si>
-  <si>
-    <t>Solicitó informes del proyecto y cotización de departamentos de 2 recamaras. Se le envió cotización del 205B. Seguimiento</t>
-  </si>
-  <si>
-    <t>Solicito información general por whats.</t>
-  </si>
-  <si>
-    <t>Fuera de presupuesto trae $4,500,000</t>
-  </si>
-  <si>
-    <t>No contesta, entra buzón. Se le envió mail de presentación y cotizaciones de 2 y 3 recamaras.
+    <t>No contesta se le envía información por mail.</t>
+  </si>
+  <si>
+    <t>Solicitó informes de departamento de 2 recamaras. se le envió el 205A.
 Seguimiento</t>
   </si>
   <si>
-    <t>Me solicitó informes de PH's: PH02A, PU06A, PH09A y PH10A</t>
-  </si>
-  <si>
-    <t>Entra buzón a la primera. Se le envió mail de presentación y cotizaciones de 2 y 3 recamaras.
+    <t>No contesta, entra buzón. Se le envió mail de presentación y cotizaciones.
+Seguimiento.</t>
+  </si>
+  <si>
+    <t>Busca en Renta de $15,000 pesos</t>
+  </si>
+  <si>
+    <t>Me contestó y me pidió cotización de 3 recamaras, se le envió el 403C
+Seguimiento.</t>
+  </si>
+  <si>
+    <t>Fuera de presupuesto $4,500,000</t>
+  </si>
+  <si>
+    <t>No dejó teléfono se le envía información general por mail</t>
+  </si>
+  <si>
+    <t>Me pidió información general no me dijo de que presupuesto. le envié de 2 y 3 recamaras.
 Seguimiento</t>
   </si>
   <si>
-    <t>Busca en Renta</t>
-  </si>
-  <si>
-    <t>Buzón de voz, se le envía información general por mail.</t>
-  </si>
-  <si>
-    <t>No dejo No. telefónico. Se le envía mail de presentación y cotización de 2 y 3 recamaras.
-Seguimiento por mail</t>
-  </si>
-  <si>
-    <t>El teléfono no sta disponible, se envía información general por mail.</t>
-  </si>
-  <si>
-    <t>No contesta, entra buzón. Se le envió mail de presentación y cotización de 2 y 3 recamaras. Seguimiento</t>
-  </si>
-  <si>
-    <t>Se les envía información de 2 y 3 recamaras a ella y a su esposo Diego Castillo</t>
-  </si>
-  <si>
-    <t>Me contacta para pedir mi iopinión sobre otros desarrollos que ha visto en Condesa y Roma, le ofrezco también Av Napoles</t>
-  </si>
-  <si>
-    <t>Cuelga el teléfono, se le envía información general por whats y por mail</t>
-  </si>
-  <si>
-    <t>Busca departamento exterior de 2 recamaras se le enviaron los modelos 8C y 8A.
+    <t>Busca para renta</t>
+  </si>
+  <si>
+    <t>Se le envía información por mail de 3 recámaras.</t>
+  </si>
+  <si>
+    <t>No contesta, entra buzón. Se le envió mail de presentación y cotizaciones. Seguimiento</t>
+  </si>
+  <si>
+    <t>Se le envía infomación de 2 recámaras mas estudio y de 3 rfecamaras mas estudio.por mail y por whats.</t>
+  </si>
+  <si>
+    <t>Le llamé y me pidió le llame en la tarde.
 Seguimiento</t>
   </si>
   <si>
-    <t>Se le envía información de 2 recamaras por whats</t>
-  </si>
-  <si>
-    <t>Entra buzón a la primera, se le envió mail de presentación y cotizaciones de 2 y 3 recamaras.</t>
-  </si>
-  <si>
-    <t>Me colgó a mitad de la llamada.</t>
-  </si>
-  <si>
-    <t>El telefono que dejo solo cuenta con servicio para navegar en internet  5513841692, se envia informacion por mail</t>
-  </si>
-  <si>
-    <t>No dejo teléfono, se le envió mail de presentación y cotización de 2 y 3 recamaras.</t>
-  </si>
-  <si>
-    <t>Se le envía información general por whats de 2 y 3 recamaras</t>
-  </si>
-  <si>
-    <t>Quieren vender su casa en los Cabos y venirse a vivir a México se le envió información de 2 y 3 recamaras por whats.</t>
-  </si>
-  <si>
-    <t>Llamada Whatsapp. Se le envía información de 2 y de 3 recamaras.</t>
-  </si>
-  <si>
-    <t>Llamada Whatsapp. 
-Solicita información, por whatsapp departamento 307A.</t>
-  </si>
-  <si>
-    <t>No lo gro comunicarme, se le envió mail de presentación y cotizaciones de 2 y 3 recamaras.</t>
-  </si>
-  <si>
-    <t>13 - 19 de Abril del 2020</t>
-  </si>
-  <si>
-    <t>No contesta, Se le envía información general por whats y por mail</t>
-  </si>
-  <si>
-    <t>Se le envia información por whatsapp departamentos de 3 recamaras.</t>
-  </si>
-  <si>
-    <t>Se le envía brochure digital e información general por mail</t>
-  </si>
-  <si>
-    <t>Andres Michel Rodrígez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ana cristina martinez </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martini </t>
+    <t>Entra buzón le envie información por mail</t>
+  </si>
+  <si>
+    <t>No contesta, entra buzón. Se le envió mail de presentación y cotizaciones.
+Seguimiento</t>
+  </si>
+  <si>
+    <t>Busca en renta, le ofrecí en venta y para poder comprar solo cuenta con $4,000,000 de pesos</t>
+  </si>
+  <si>
+    <t>No dejo numero telefónico, se le envió mail de presentación y cotizaciones.
+Seguimiento</t>
+  </si>
+  <si>
+    <t>Se le envía información de 2 recámaras por whats</t>
+  </si>
+  <si>
+    <t>Dejó teléfono equivocado, se le envió mail de presentación y cotizaciones.</t>
+  </si>
+  <si>
+    <t>Fuera de presupuesto trae $4,000,000</t>
+  </si>
+  <si>
+    <t>Se le dejo mensaje a su contestadora, también se le envió mail de presentación y cotizaciones.
+Seguimientos</t>
+  </si>
+  <si>
+    <t>Entra buzón, se le envió mail de presentación y cotizaciones.
+Seguimiento</t>
+  </si>
+  <si>
+    <t>20 - 26 de Abril del 2020</t>
+  </si>
+  <si>
+    <t>No contesta se le envía información general por mail y se le envía whats App</t>
+  </si>
+  <si>
+    <t>Arturo Joya Cantor</t>
+  </si>
+  <si>
+    <t>Solicita información general, que si hay interes me llama, daré seguimiento</t>
+  </si>
+  <si>
+    <t>No contesta, se le envia mail de presentación y cotización de dos y tres recámaras, Seguimiento</t>
+  </si>
+  <si>
+    <t>Solicita información general y cotización de dos recámaras, se le envió cotización de 205B</t>
+  </si>
+  <si>
+    <t>Solicita información general y cotización de dos y tres recámaras, se le envió cotización de 205B y 403C Seguimiento</t>
   </si>
 </sst>
 </file>
@@ -950,13 +926,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1054100</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1257300</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>203258</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1294,10 +1270,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A4:L253"/>
+  <dimension ref="A4:L251"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1309,7 +1285,7 @@
     <col min="5" max="5" width="14.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="34.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30" style="2" customWidth="1"/>
+    <col min="8" max="8" width="46.83203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="132.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="94.5" style="1" customWidth="1"/>
     <col min="11" max="12" width="10.6640625" style="1" customWidth="1"/>
@@ -1344,7 +1320,7 @@
     </row>
     <row r="15" spans="2:10" ht="23" x14ac:dyDescent="0.35">
       <c r="B15" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="8"/>
@@ -1353,7 +1329,7 @@
     </row>
     <row r="16" spans="2:10" ht="23" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="8"/>
@@ -1369,7 +1345,7 @@
     </row>
     <row r="18" spans="2:9" ht="20" x14ac:dyDescent="0.25">
       <c r="B18" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="12"/>
@@ -1385,13 +1361,13 @@
     </row>
     <row r="20" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B20" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="34">
+        <v>38</v>
+      </c>
+      <c r="E20" s="33" t="s">
         <v>20</v>
-      </c>
-      <c r="C20" s="34">
-        <v>40</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>21</v>
       </c>
       <c r="F20" s="34">
         <v>0</v>
@@ -1404,10 +1380,10 @@
       <c r="B21" s="31"/>
       <c r="C21" s="32"/>
       <c r="E21" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="31"/>
@@ -1417,10 +1393,10 @@
       <c r="B22" s="31"/>
       <c r="C22" s="32"/>
       <c r="E22" s="33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="34">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="31"/>
@@ -1430,7 +1406,7 @@
       <c r="B23" s="31"/>
       <c r="C23" s="32"/>
       <c r="E23" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F23" s="34">
         <v>22</v>
@@ -1450,16 +1426,16 @@
     </row>
     <row r="25" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B25" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="34">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E25" s="33" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="34">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="9"/>
@@ -1467,33 +1443,29 @@
     </row>
     <row r="26" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B26" s="37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="34">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F26" s="34">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="9"/>
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="2:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="B27" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="34">
-        <v>1</v>
-      </c>
+      <c r="B27" s="39"/>
+      <c r="C27" s="34"/>
       <c r="E27" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F27" s="34">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="9"/>
@@ -1503,7 +1475,7 @@
       <c r="B28" s="31"/>
       <c r="C28" s="32"/>
       <c r="E28" s="33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F28" s="34">
         <v>0</v>
@@ -1515,7 +1487,7 @@
     <row r="29" spans="2:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B29" s="31"/>
       <c r="E29" s="33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F29" s="34">
         <v>0</v>
@@ -1533,7 +1505,7 @@
     </row>
     <row r="31" spans="2:9" ht="20" x14ac:dyDescent="0.25">
       <c r="B31" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="12"/>
@@ -1558,7 +1530,7 @@
         <v>8</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F33" s="13" t="s">
         <v>9</v>
@@ -1578,26 +1550,28 @@
         <v>1</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F34" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="G34" s="39"/>
+        <v>71</v>
+      </c>
+      <c r="G34" s="39">
+        <v>5544994107</v>
+      </c>
       <c r="H34" s="39" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="I34" s="39" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.25">
@@ -1605,28 +1579,28 @@
         <v>2</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="F35" s="39" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G35" s="39">
-        <v>5614005671</v>
+        <v>5510090332</v>
       </c>
       <c r="H35" s="39" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="I35" s="39" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1634,10 +1608,10 @@
         <v>3</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D36" s="38" t="s">
         <v>3</v>
@@ -1646,16 +1620,16 @@
         <v>13</v>
       </c>
       <c r="F36" s="39" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="G36" s="39">
-        <v>5541426527</v>
+        <v>7472543976</v>
       </c>
       <c r="H36" s="39" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="I36" s="39" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1663,10 +1637,10 @@
         <v>4</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="D37" s="38" t="s">
         <v>3</v>
@@ -1675,16 +1649,16 @@
         <v>13</v>
       </c>
       <c r="F37" s="39" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="G37" s="39">
-        <v>5523196455</v>
+        <v>5532007809</v>
       </c>
       <c r="H37" s="39" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="I37" s="39" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1692,10 +1666,10 @@
         <v>5</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D38" s="38" t="s">
         <v>3</v>
@@ -1704,16 +1678,16 @@
         <v>13</v>
       </c>
       <c r="F38" s="39" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="G38" s="39">
-        <v>6241540611</v>
+        <v>5532000100</v>
       </c>
       <c r="H38" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="I38" s="39" t="s">
         <v>148</v>
-      </c>
-      <c r="I38" s="39" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1724,25 +1698,25 @@
         <v>29</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D39" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="39" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="F39" s="39" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G39" s="39">
-        <v>7122247200</v>
+        <v>5534007613</v>
       </c>
       <c r="H39" s="39" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="I39" s="39" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1753,25 +1727,25 @@
         <v>29</v>
       </c>
       <c r="C40" s="39" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D40" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E40" s="39" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="F40" s="39" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="G40" s="39">
-        <v>5512353638</v>
+        <v>9932781335</v>
       </c>
       <c r="H40" s="39" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="I40" s="39" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1779,28 +1753,28 @@
         <v>8</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C41" s="39" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="D41" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F41" s="39" t="s">
-        <v>189</v>
+        <v>73</v>
       </c>
       <c r="G41" s="39">
-        <v>5536599923</v>
+        <v>5527066947</v>
       </c>
       <c r="H41" s="39" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="I41" s="39" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1808,28 +1782,28 @@
         <v>9</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C42" s="39" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D42" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E42" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F42" s="39" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G42" s="39">
-        <v>5580664676</v>
+        <v>5539911426</v>
       </c>
       <c r="H42" s="39" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="I42" s="39" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1837,28 +1811,28 @@
         <v>10</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D43" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E43" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F43" s="39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G43" s="39">
-        <v>5586180506</v>
+        <v>5565434658</v>
       </c>
       <c r="H43" s="39" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I43" s="39" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1866,28 +1840,28 @@
         <v>11</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C44" s="39" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D44" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E44" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F44" s="39" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G44" s="39">
-        <v>5527656800</v>
+        <v>5561114476</v>
       </c>
       <c r="H44" s="39" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I44" s="39" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1895,28 +1869,26 @@
         <v>12</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C45" s="39" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D45" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F45" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="G45" s="39">
-        <v>7712196127</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="G45" s="39"/>
       <c r="H45" s="39" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="I45" s="39" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1924,28 +1896,28 @@
         <v>13</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C46" s="39" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D46" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E46" s="39" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F46" s="39" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G46" s="39">
-        <v>5539334916</v>
+        <v>5519784585</v>
       </c>
       <c r="H46" s="39" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I46" s="39" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1956,25 +1928,25 @@
         <v>29</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D47" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E47" s="39" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F47" s="39" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="G47" s="39">
-        <v>5534199158</v>
+        <v>5513302253</v>
       </c>
       <c r="H47" s="39" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="I47" s="39" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="J47" s="12"/>
     </row>
@@ -1983,28 +1955,28 @@
         <v>15</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C48" s="39" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D48" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E48" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F48" s="39" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="G48" s="39">
-        <v>5533967102</v>
+        <v>5543687556</v>
       </c>
       <c r="H48" s="39" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="I48" s="39" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2012,28 +1984,26 @@
         <v>16</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C49" s="39" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D49" s="38" t="s">
         <v>3</v>
       </c>
       <c r="E49" s="39" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F49" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="G49" s="39">
-        <v>5530350424</v>
-      </c>
+      <c r="G49" s="39"/>
       <c r="H49" s="39" t="s">
         <v>124</v>
       </c>
       <c r="I49" s="39" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2041,28 +2011,28 @@
         <v>17</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C50" s="39" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E50" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F50" s="39" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="G50" s="39">
-        <v>6413228237</v>
+        <v>5533762310</v>
       </c>
       <c r="H50" s="39" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="I50" s="39" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2070,28 +2040,28 @@
         <v>18</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C51" s="39" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D51" s="38" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E51" s="39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F51" s="39" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G51" s="39">
-        <v>5525609124</v>
+        <v>8182532698</v>
       </c>
       <c r="H51" s="39" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="I51" s="39" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2099,28 +2069,28 @@
         <v>19</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C52" s="39" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="D52" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E52" s="39" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F52" s="39" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="G52" s="39">
-        <v>41738560</v>
+        <v>8120211497</v>
       </c>
       <c r="H52" s="39" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="I52" s="39" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2128,28 +2098,26 @@
         <v>20</v>
       </c>
       <c r="B53" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C53" s="39" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="D53" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E53" s="39" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F53" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="G53" s="39">
-        <v>5554376496</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="G53" s="39"/>
       <c r="H53" s="39" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="I53" s="39" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2157,28 +2125,28 @@
         <v>21</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C54" s="39" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="D54" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E54" s="39" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F54" s="39" t="s">
-        <v>89</v>
+        <v>178</v>
       </c>
       <c r="G54" s="39">
-        <v>5518471074</v>
+        <v>5553630110</v>
       </c>
       <c r="H54" s="39" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="I54" s="39" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2189,23 +2157,23 @@
         <v>29</v>
       </c>
       <c r="C55" s="39" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="D55" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E55" s="39" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F55" s="39" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G55" s="39"/>
       <c r="H55" s="39" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="I55" s="39" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2213,10 +2181,10 @@
         <v>23</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C56" s="39" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D56" s="38" t="s">
         <v>5</v>
@@ -2225,16 +2193,16 @@
         <v>13</v>
       </c>
       <c r="F56" s="39" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="G56" s="39">
-        <v>5519515706</v>
+        <v>5543666020</v>
       </c>
       <c r="H56" s="39" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="I56" s="39" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2242,10 +2210,10 @@
         <v>24</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C57" s="39" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D57" s="38" t="s">
         <v>5</v>
@@ -2254,16 +2222,16 @@
         <v>13</v>
       </c>
       <c r="F57" s="39" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="G57" s="39">
-        <v>5523004330</v>
+        <v>6181569677</v>
       </c>
       <c r="H57" s="39" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="I57" s="39" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2271,10 +2239,10 @@
         <v>25</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C58" s="39" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D58" s="38" t="s">
         <v>5</v>
@@ -2283,16 +2251,16 @@
         <v>13</v>
       </c>
       <c r="F58" s="39" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G58" s="39">
-        <v>5569006106</v>
+        <v>6644031020</v>
       </c>
       <c r="H58" s="39" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="I58" s="39" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2300,10 +2268,10 @@
         <v>26</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C59" s="39" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="D59" s="38" t="s">
         <v>5</v>
@@ -2312,16 +2280,16 @@
         <v>13</v>
       </c>
       <c r="F59" s="39" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="G59" s="39">
-        <v>5513335213</v>
+        <v>5554371660</v>
       </c>
       <c r="H59" s="39" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="I59" s="39" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2329,10 +2297,10 @@
         <v>27</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C60" s="39" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="D60" s="38" t="s">
         <v>5</v>
@@ -2341,16 +2309,16 @@
         <v>13</v>
       </c>
       <c r="F60" s="39" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="G60" s="39">
-        <v>4442013260</v>
+        <v>556677887788</v>
       </c>
       <c r="H60" s="39" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="I60" s="39" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2358,10 +2326,10 @@
         <v>28</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C61" s="39" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="D61" s="38" t="s">
         <v>5</v>
@@ -2370,16 +2338,16 @@
         <v>13</v>
       </c>
       <c r="F61" s="39" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="G61" s="39">
-        <v>5512965912</v>
+        <v>5532245571</v>
       </c>
       <c r="H61" s="39" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="I61" s="39" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2387,28 +2355,28 @@
         <v>29</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C62" s="39" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D62" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E62" s="39" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F62" s="39" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="G62" s="39">
-        <v>5548998870</v>
+        <v>5527446861</v>
       </c>
       <c r="H62" s="39" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="I62" s="39" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2416,28 +2384,28 @@
         <v>30</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C63" s="39" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D63" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E63" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F63" s="39" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="G63" s="39">
-        <v>5516821634</v>
+        <v>525620153702</v>
       </c>
       <c r="H63" s="39" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="I63" s="39" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2445,28 +2413,28 @@
         <v>31</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C64" s="39" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D64" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E64" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F64" s="39" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G64" s="39">
-        <v>7225336736</v>
+        <v>4422009133</v>
       </c>
       <c r="H64" s="39" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I64" s="39" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2477,25 +2445,25 @@
         <v>29</v>
       </c>
       <c r="C65" s="39" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D65" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F65" s="39" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="G65" s="39">
-        <v>6624717691</v>
+        <v>9612737489</v>
       </c>
       <c r="H65" s="39" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="I65" s="39" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2506,25 +2474,25 @@
         <v>29</v>
       </c>
       <c r="C66" s="39" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="D66" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E66" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F66" s="39" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="G66" s="39">
-        <v>4499119282</v>
+        <v>4448275239</v>
       </c>
       <c r="H66" s="39" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="I66" s="39" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2535,23 +2503,25 @@
         <v>29</v>
       </c>
       <c r="C67" s="39" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D67" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E67" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F67" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="G67" s="39"/>
+        <v>84</v>
+      </c>
+      <c r="G67" s="39">
+        <v>5579035099</v>
+      </c>
       <c r="H67" s="39" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="I67" s="39" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2562,25 +2532,25 @@
         <v>29</v>
       </c>
       <c r="C68" s="39" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D68" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E68" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F68" s="39" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="G68" s="39">
-        <v>5538853148</v>
+        <v>5535002812</v>
       </c>
       <c r="H68" s="39" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="I68" s="39" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="17" x14ac:dyDescent="0.25">
@@ -2588,28 +2558,26 @@
         <v>36</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C69" s="39" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D69" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E69" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F69" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="G69" s="39">
-        <v>5564150057</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="G69" s="39"/>
       <c r="H69" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I69" s="39" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="17" x14ac:dyDescent="0.25">
@@ -2617,28 +2585,28 @@
         <v>37</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C70" s="39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D70" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E70" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F70" s="39" t="s">
-        <v>190</v>
+        <v>93</v>
       </c>
       <c r="G70" s="39">
-        <v>5560707606</v>
+        <v>3467004615</v>
       </c>
       <c r="H70" s="39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I70" s="39" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="17" x14ac:dyDescent="0.25">
@@ -2646,112 +2614,74 @@
         <v>38</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C71" s="39" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D71" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E71" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F71" s="39" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G71" s="39">
-        <v>5579243781</v>
+        <v>5578467984</v>
       </c>
       <c r="H71" s="39" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="I71" s="39" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>39</v>
-      </c>
-      <c r="B72" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C72" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="D72" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E72" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F72" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="G72" s="39">
-        <v>9512338043</v>
-      </c>
-      <c r="H72" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="I72" s="39" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="17" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>40</v>
-      </c>
-      <c r="B73" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C73" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D73" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E73" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F73" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="G73" s="39">
-        <v>13841692</v>
-      </c>
-      <c r="H73" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="I73" s="39" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="11" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="39"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="38"/>
-      <c r="F74" s="38"/>
-      <c r="G74" s="41"/>
-      <c r="H74" s="42"/>
-      <c r="I74" s="41"/>
-    </row>
-    <row r="75" spans="1:9" ht="11" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="39"/>
-      <c r="C75" s="40"/>
-      <c r="D75" s="38"/>
-      <c r="E75" s="38"/>
-      <c r="F75" s="38"/>
-      <c r="G75" s="41"/>
-      <c r="H75" s="42"/>
-      <c r="I75" s="41"/>
-    </row>
-    <row r="76" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="36" t="s">
-        <v>17</v>
-      </c>
+    <row r="72" spans="1:9" ht="11" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="39"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="38"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="41"/>
+      <c r="H72" s="42"/>
+      <c r="I72" s="41"/>
+    </row>
+    <row r="73" spans="1:9" ht="11" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="39"/>
+      <c r="C73" s="40"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="41"/>
+      <c r="H73" s="42"/>
+      <c r="I73" s="41"/>
+    </row>
+    <row r="74" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" s="19"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="20"/>
+      <c r="I74" s="12"/>
+    </row>
+    <row r="75" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="18"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="20"/>
+      <c r="I75" s="12"/>
+    </row>
+    <row r="76" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="18"/>
       <c r="C76" s="19"/>
       <c r="D76" s="18"/>
       <c r="E76" s="18"/>
@@ -2761,31 +2691,39 @@
       <c r="I76" s="12"/>
     </row>
     <row r="77" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="18"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="20"/>
+      <c r="B77" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77" s="24"/>
+      <c r="E77" s="25"/>
+      <c r="F77" s="26"/>
+      <c r="G77" s="27"/>
+      <c r="H77" s="28"/>
       <c r="I77" s="12"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="18"/>
-      <c r="C78" s="19"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="20"/>
+      <c r="B78" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D78" s="24"/>
+      <c r="E78" s="25"/>
+      <c r="F78" s="26"/>
+      <c r="G78" s="27"/>
+      <c r="H78" s="28"/>
       <c r="I78" s="12"/>
     </row>
     <row r="79" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="22" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C79" s="23" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D79" s="24"/>
       <c r="E79" s="25"/>
@@ -2794,49 +2732,39 @@
       <c r="H79" s="28"/>
       <c r="I79" s="12"/>
     </row>
-    <row r="80" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="B80" s="22" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D80" s="24"/>
       <c r="E80" s="25"/>
-      <c r="F80" s="26"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="28"/>
-      <c r="I80" s="12"/>
-    </row>
-    <row r="81" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C81" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D81" s="24"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="26"/>
-      <c r="G81" s="27"/>
-      <c r="H81" s="28"/>
-      <c r="I81" s="12"/>
-    </row>
-    <row r="82" spans="2:12" ht="17" x14ac:dyDescent="0.25">
-      <c r="B82" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D82" s="24"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
-      <c r="G82" s="29"/>
-      <c r="H82" s="30"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="29"/>
+      <c r="H80" s="30"/>
+      <c r="I80" s="6"/>
+    </row>
+    <row r="81" spans="2:12" ht="16" x14ac:dyDescent="0.25">
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="6"/>
+      <c r="I81" s="6"/>
+    </row>
+    <row r="82" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="6"/>
       <c r="I82" s="6"/>
     </row>
-    <row r="83" spans="2:12" ht="16" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
@@ -2844,6 +2772,7 @@
       <c r="F83" s="5"/>
       <c r="G83" s="6"/>
       <c r="I83" s="6"/>
+      <c r="J83" s="21"/>
     </row>
     <row r="84" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="6"/>
@@ -2853,8 +2782,9 @@
       <c r="F84" s="5"/>
       <c r="G84" s="6"/>
       <c r="I84" s="6"/>
-    </row>
-    <row r="85" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J84" s="21"/>
+    </row>
+    <row r="85" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
@@ -2865,7 +2795,9 @@
       <c r="J85" s="21"/>
     </row>
     <row r="86" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="6"/>
+      <c r="B86" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
@@ -2874,7 +2806,7 @@
       <c r="I86" s="6"/>
       <c r="J86" s="21"/>
     </row>
-    <row r="87" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
@@ -2885,15 +2817,14 @@
       <c r="J87" s="21"/>
     </row>
     <row r="88" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="6"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="6"/>
-      <c r="I88" s="6"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="3"/>
       <c r="J88" s="21"/>
     </row>
     <row r="89" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2907,14 +2838,13 @@
       <c r="J89" s="21"/>
     </row>
     <row r="90" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-      <c r="H90" s="4"/>
-      <c r="I90" s="3"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="6"/>
+      <c r="I90" s="6"/>
       <c r="J90" s="21"/>
     </row>
     <row r="91" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2925,7 +2855,9 @@
       <c r="F91" s="5"/>
       <c r="G91" s="6"/>
       <c r="I91" s="6"/>
-      <c r="J91" s="21"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
     </row>
     <row r="92" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="6"/>
@@ -2935,7 +2867,9 @@
       <c r="F92" s="5"/>
       <c r="G92" s="6"/>
       <c r="I92" s="6"/>
-      <c r="J92" s="21"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="6"/>
     </row>
     <row r="93" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="6"/>
@@ -3017,7 +2951,7 @@
       <c r="F99" s="5"/>
       <c r="G99" s="6"/>
       <c r="I99" s="6"/>
-      <c r="J99" s="6"/>
+      <c r="J99" s="3"/>
       <c r="K99" s="6"/>
       <c r="L99" s="6"/>
     </row>
@@ -3041,7 +2975,7 @@
       <c r="F101" s="5"/>
       <c r="G101" s="6"/>
       <c r="I101" s="6"/>
-      <c r="J101" s="3"/>
+      <c r="J101" s="6"/>
       <c r="K101" s="6"/>
       <c r="L101" s="6"/>
     </row>
@@ -4713,87 +4647,63 @@
       <c r="K240" s="6"/>
       <c r="L240" s="6"/>
     </row>
-    <row r="241" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B241" s="6"/>
-      <c r="C241" s="6"/>
-      <c r="D241" s="6"/>
-      <c r="E241" s="6"/>
-      <c r="F241" s="5"/>
-      <c r="G241" s="6"/>
-      <c r="I241" s="6"/>
+    <row r="241" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J241" s="6"/>
       <c r="K241" s="6"/>
       <c r="L241" s="6"/>
     </row>
-    <row r="242" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B242" s="6"/>
-      <c r="C242" s="6"/>
-      <c r="D242" s="6"/>
-      <c r="E242" s="6"/>
-      <c r="F242" s="5"/>
-      <c r="G242" s="6"/>
-      <c r="I242" s="6"/>
+    <row r="242" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J242" s="6"/>
       <c r="K242" s="6"/>
       <c r="L242" s="6"/>
     </row>
-    <row r="243" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J243" s="6"/>
       <c r="K243" s="6"/>
       <c r="L243" s="6"/>
     </row>
-    <row r="244" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J244" s="6"/>
       <c r="K244" s="6"/>
       <c r="L244" s="6"/>
     </row>
-    <row r="245" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J245" s="6"/>
       <c r="K245" s="6"/>
       <c r="L245" s="6"/>
     </row>
-    <row r="246" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J246" s="6"/>
       <c r="K246" s="6"/>
       <c r="L246" s="6"/>
     </row>
-    <row r="247" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J247" s="6"/>
       <c r="K247" s="6"/>
       <c r="L247" s="6"/>
     </row>
-    <row r="248" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J248" s="6"/>
       <c r="K248" s="6"/>
       <c r="L248" s="6"/>
     </row>
-    <row r="249" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J249" s="6"/>
       <c r="K249" s="6"/>
       <c r="L249" s="6"/>
     </row>
-    <row r="250" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J250" s="6"/>
       <c r="K250" s="6"/>
       <c r="L250" s="6"/>
     </row>
-    <row r="251" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="10:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J251" s="6"/>
       <c r="K251" s="6"/>
       <c r="L251" s="6"/>
     </row>
-    <row r="252" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J252" s="6"/>
-      <c r="K252" s="6"/>
-      <c r="L252" s="6"/>
-    </row>
-    <row r="253" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J253" s="6"/>
-      <c r="K253" s="6"/>
-      <c r="L253" s="6"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:A73">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A34:A71">
     <sortCondition ref="A34"/>
   </sortState>
   <printOptions horizontalCentered="1"/>

</xml_diff>